<commit_message>
Project Plan & RTM updated
Signed-off-by: NorhanNassar <norhan.nassar96@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PP.xlsx
+++ b/SW deliveries log/PP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7548" yWindow="0" windowWidth="21504" windowHeight="9780" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="8952" yWindow="0" windowWidth="21504" windowHeight="9780" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Gantt Chart - EX" sheetId="1" r:id="rId1"/>
@@ -1298,7 +1298,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1535,12 +1535,88 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="8" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="23" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1553,82 +1629,9 @@
     <xf numFmtId="0" fontId="4" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="8" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -1986,74 +1989,74 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="114" t="s">
+      <c r="I7" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="115"/>
-      <c r="K7" s="115"/>
-      <c r="L7" s="115"/>
-      <c r="M7" s="115"/>
-      <c r="N7" s="115"/>
-      <c r="O7" s="115"/>
-      <c r="P7" s="115"/>
-      <c r="Q7" s="115"/>
-      <c r="R7" s="115"/>
-      <c r="S7" s="115"/>
-      <c r="T7" s="115"/>
-      <c r="U7" s="115"/>
-      <c r="V7" s="115"/>
-      <c r="W7" s="116"/>
-      <c r="X7" s="108" t="s">
+      <c r="J7" s="116"/>
+      <c r="K7" s="116"/>
+      <c r="L7" s="116"/>
+      <c r="M7" s="116"/>
+      <c r="N7" s="116"/>
+      <c r="O7" s="116"/>
+      <c r="P7" s="116"/>
+      <c r="Q7" s="116"/>
+      <c r="R7" s="116"/>
+      <c r="S7" s="116"/>
+      <c r="T7" s="116"/>
+      <c r="U7" s="116"/>
+      <c r="V7" s="116"/>
+      <c r="W7" s="117"/>
+      <c r="X7" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="Y7" s="109"/>
-      <c r="Z7" s="109"/>
-      <c r="AA7" s="109"/>
-      <c r="AB7" s="109"/>
-      <c r="AC7" s="109"/>
-      <c r="AD7" s="109"/>
-      <c r="AE7" s="109"/>
-      <c r="AF7" s="109"/>
-      <c r="AG7" s="109"/>
-      <c r="AH7" s="109"/>
-      <c r="AI7" s="109"/>
-      <c r="AJ7" s="109"/>
-      <c r="AK7" s="109"/>
-      <c r="AL7" s="110"/>
-      <c r="AM7" s="111" t="s">
+      <c r="Y7" s="110"/>
+      <c r="Z7" s="110"/>
+      <c r="AA7" s="110"/>
+      <c r="AB7" s="110"/>
+      <c r="AC7" s="110"/>
+      <c r="AD7" s="110"/>
+      <c r="AE7" s="110"/>
+      <c r="AF7" s="110"/>
+      <c r="AG7" s="110"/>
+      <c r="AH7" s="110"/>
+      <c r="AI7" s="110"/>
+      <c r="AJ7" s="110"/>
+      <c r="AK7" s="110"/>
+      <c r="AL7" s="111"/>
+      <c r="AM7" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="AN7" s="112"/>
-      <c r="AO7" s="112"/>
-      <c r="AP7" s="112"/>
-      <c r="AQ7" s="112"/>
-      <c r="AR7" s="112"/>
-      <c r="AS7" s="112"/>
-      <c r="AT7" s="112"/>
-      <c r="AU7" s="112"/>
-      <c r="AV7" s="112"/>
-      <c r="AW7" s="112"/>
-      <c r="AX7" s="112"/>
-      <c r="AY7" s="112"/>
-      <c r="AZ7" s="112"/>
-      <c r="BA7" s="113"/>
-      <c r="BB7" s="117" t="s">
+      <c r="AN7" s="113"/>
+      <c r="AO7" s="113"/>
+      <c r="AP7" s="113"/>
+      <c r="AQ7" s="113"/>
+      <c r="AR7" s="113"/>
+      <c r="AS7" s="113"/>
+      <c r="AT7" s="113"/>
+      <c r="AU7" s="113"/>
+      <c r="AV7" s="113"/>
+      <c r="AW7" s="113"/>
+      <c r="AX7" s="113"/>
+      <c r="AY7" s="113"/>
+      <c r="AZ7" s="113"/>
+      <c r="BA7" s="114"/>
+      <c r="BB7" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="BC7" s="118"/>
-      <c r="BD7" s="118"/>
-      <c r="BE7" s="118"/>
-      <c r="BF7" s="118"/>
-      <c r="BG7" s="118"/>
-      <c r="BH7" s="118"/>
-      <c r="BI7" s="118"/>
-      <c r="BJ7" s="118"/>
-      <c r="BK7" s="118"/>
-      <c r="BL7" s="118"/>
-      <c r="BM7" s="118"/>
-      <c r="BN7" s="118"/>
-      <c r="BO7" s="118"/>
-      <c r="BP7" s="119"/>
+      <c r="BC7" s="119"/>
+      <c r="BD7" s="119"/>
+      <c r="BE7" s="119"/>
+      <c r="BF7" s="119"/>
+      <c r="BG7" s="119"/>
+      <c r="BH7" s="119"/>
+      <c r="BI7" s="119"/>
+      <c r="BJ7" s="119"/>
+      <c r="BK7" s="119"/>
+      <c r="BL7" s="119"/>
+      <c r="BM7" s="119"/>
+      <c r="BN7" s="119"/>
+      <c r="BO7" s="119"/>
+      <c r="BP7" s="120"/>
     </row>
     <row r="8" spans="2:68" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
@@ -2077,90 +2080,90 @@
       <c r="H8" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="126" t="s">
+      <c r="I8" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="124"/>
-      <c r="K8" s="124"/>
-      <c r="L8" s="124"/>
-      <c r="M8" s="124"/>
-      <c r="N8" s="124" t="s">
+      <c r="J8" s="126"/>
+      <c r="K8" s="126"/>
+      <c r="L8" s="126"/>
+      <c r="M8" s="126"/>
+      <c r="N8" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="O8" s="124"/>
-      <c r="P8" s="124"/>
-      <c r="Q8" s="124"/>
-      <c r="R8" s="124"/>
-      <c r="S8" s="124" t="s">
+      <c r="O8" s="126"/>
+      <c r="P8" s="126"/>
+      <c r="Q8" s="126"/>
+      <c r="R8" s="126"/>
+      <c r="S8" s="126" t="s">
         <v>7</v>
       </c>
-      <c r="T8" s="124"/>
-      <c r="U8" s="124"/>
-      <c r="V8" s="124"/>
-      <c r="W8" s="125"/>
-      <c r="X8" s="105" t="s">
+      <c r="T8" s="126"/>
+      <c r="U8" s="126"/>
+      <c r="V8" s="126"/>
+      <c r="W8" s="127"/>
+      <c r="X8" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="Y8" s="106"/>
-      <c r="Z8" s="106"/>
-      <c r="AA8" s="106"/>
-      <c r="AB8" s="106"/>
-      <c r="AC8" s="106" t="s">
+      <c r="Y8" s="132"/>
+      <c r="Z8" s="132"/>
+      <c r="AA8" s="132"/>
+      <c r="AB8" s="132"/>
+      <c r="AC8" s="132" t="s">
         <v>9</v>
       </c>
-      <c r="AD8" s="106"/>
-      <c r="AE8" s="106"/>
-      <c r="AF8" s="106"/>
-      <c r="AG8" s="106"/>
-      <c r="AH8" s="106" t="s">
+      <c r="AD8" s="132"/>
+      <c r="AE8" s="132"/>
+      <c r="AF8" s="132"/>
+      <c r="AG8" s="132"/>
+      <c r="AH8" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="AI8" s="106"/>
-      <c r="AJ8" s="106"/>
-      <c r="AK8" s="106"/>
-      <c r="AL8" s="107"/>
-      <c r="AM8" s="102" t="s">
+      <c r="AI8" s="132"/>
+      <c r="AJ8" s="132"/>
+      <c r="AK8" s="132"/>
+      <c r="AL8" s="133"/>
+      <c r="AM8" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="AN8" s="103"/>
-      <c r="AO8" s="103"/>
-      <c r="AP8" s="103"/>
-      <c r="AQ8" s="103"/>
-      <c r="AR8" s="103" t="s">
+      <c r="AN8" s="121"/>
+      <c r="AO8" s="121"/>
+      <c r="AP8" s="121"/>
+      <c r="AQ8" s="121"/>
+      <c r="AR8" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="AS8" s="103"/>
-      <c r="AT8" s="103"/>
-      <c r="AU8" s="103"/>
-      <c r="AV8" s="103"/>
-      <c r="AW8" s="103" t="s">
+      <c r="AS8" s="121"/>
+      <c r="AT8" s="121"/>
+      <c r="AU8" s="121"/>
+      <c r="AV8" s="121"/>
+      <c r="AW8" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="AX8" s="103"/>
-      <c r="AY8" s="103"/>
-      <c r="AZ8" s="103"/>
-      <c r="BA8" s="120"/>
-      <c r="BB8" s="121" t="s">
+      <c r="AX8" s="121"/>
+      <c r="AY8" s="121"/>
+      <c r="AZ8" s="121"/>
+      <c r="BA8" s="122"/>
+      <c r="BB8" s="123" t="s">
         <v>14</v>
       </c>
-      <c r="BC8" s="122"/>
-      <c r="BD8" s="122"/>
-      <c r="BE8" s="122"/>
-      <c r="BF8" s="122"/>
-      <c r="BG8" s="122" t="s">
+      <c r="BC8" s="124"/>
+      <c r="BD8" s="124"/>
+      <c r="BE8" s="124"/>
+      <c r="BF8" s="124"/>
+      <c r="BG8" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="BH8" s="122"/>
-      <c r="BI8" s="122"/>
-      <c r="BJ8" s="122"/>
-      <c r="BK8" s="122"/>
-      <c r="BL8" s="122" t="s">
+      <c r="BH8" s="124"/>
+      <c r="BI8" s="124"/>
+      <c r="BJ8" s="124"/>
+      <c r="BK8" s="124"/>
+      <c r="BL8" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="BM8" s="122"/>
-      <c r="BN8" s="122"/>
-      <c r="BO8" s="122"/>
-      <c r="BP8" s="123"/>
+      <c r="BM8" s="124"/>
+      <c r="BN8" s="124"/>
+      <c r="BO8" s="124"/>
+      <c r="BP8" s="125"/>
     </row>
     <row r="9" spans="2:68" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="9" t="s">
@@ -4388,81 +4391,85 @@
       <c r="BP34" s="40"/>
     </row>
     <row r="36" spans="2:68" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="104" t="s">
+      <c r="B36" s="130" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="104"/>
-      <c r="D36" s="104"/>
-      <c r="E36" s="104"/>
-      <c r="F36" s="104"/>
-      <c r="G36" s="104"/>
-      <c r="H36" s="104"/>
-      <c r="I36" s="104"/>
-      <c r="J36" s="104"/>
-      <c r="K36" s="104"/>
-      <c r="L36" s="104"/>
-      <c r="M36" s="104"/>
-      <c r="N36" s="104"/>
-      <c r="O36" s="104"/>
-      <c r="P36" s="104"/>
-      <c r="Q36" s="104"/>
-      <c r="R36" s="104"/>
-      <c r="S36" s="104"/>
-      <c r="T36" s="104"/>
-      <c r="U36" s="104"/>
-      <c r="V36" s="104"/>
-      <c r="W36" s="104"/>
-      <c r="X36" s="104"/>
-      <c r="Y36" s="104"/>
-      <c r="Z36" s="104"/>
-      <c r="AA36" s="104"/>
-      <c r="AB36" s="104"/>
-      <c r="AC36" s="104"/>
-      <c r="AD36" s="104"/>
-      <c r="AE36" s="104"/>
-      <c r="AF36" s="104"/>
-      <c r="AG36" s="104"/>
-      <c r="AH36" s="104"/>
-      <c r="AI36" s="104"/>
-      <c r="AJ36" s="104"/>
-      <c r="AK36" s="104"/>
-      <c r="AL36" s="104"/>
-      <c r="AM36" s="104"/>
-      <c r="AN36" s="104"/>
-      <c r="AO36" s="104"/>
-      <c r="AP36" s="104"/>
-      <c r="AQ36" s="104"/>
-      <c r="AR36" s="104"/>
-      <c r="AS36" s="104"/>
-      <c r="AT36" s="104"/>
-      <c r="AU36" s="104"/>
-      <c r="AV36" s="104"/>
-      <c r="AW36" s="104"/>
-      <c r="AX36" s="104"/>
-      <c r="AY36" s="104"/>
-      <c r="AZ36" s="104"/>
-      <c r="BA36" s="104"/>
-      <c r="BB36" s="104"/>
-      <c r="BC36" s="104"/>
-      <c r="BD36" s="104"/>
-      <c r="BE36" s="104"/>
-      <c r="BF36" s="104"/>
-      <c r="BG36" s="104"/>
-      <c r="BH36" s="104"/>
-      <c r="BI36" s="104"/>
-      <c r="BJ36" s="104"/>
-      <c r="BK36" s="104"/>
-      <c r="BL36" s="104"/>
-      <c r="BM36" s="104"/>
-      <c r="BN36" s="104"/>
-      <c r="BO36" s="104"/>
-      <c r="BP36" s="104"/>
+      <c r="C36" s="130"/>
+      <c r="D36" s="130"/>
+      <c r="E36" s="130"/>
+      <c r="F36" s="130"/>
+      <c r="G36" s="130"/>
+      <c r="H36" s="130"/>
+      <c r="I36" s="130"/>
+      <c r="J36" s="130"/>
+      <c r="K36" s="130"/>
+      <c r="L36" s="130"/>
+      <c r="M36" s="130"/>
+      <c r="N36" s="130"/>
+      <c r="O36" s="130"/>
+      <c r="P36" s="130"/>
+      <c r="Q36" s="130"/>
+      <c r="R36" s="130"/>
+      <c r="S36" s="130"/>
+      <c r="T36" s="130"/>
+      <c r="U36" s="130"/>
+      <c r="V36" s="130"/>
+      <c r="W36" s="130"/>
+      <c r="X36" s="130"/>
+      <c r="Y36" s="130"/>
+      <c r="Z36" s="130"/>
+      <c r="AA36" s="130"/>
+      <c r="AB36" s="130"/>
+      <c r="AC36" s="130"/>
+      <c r="AD36" s="130"/>
+      <c r="AE36" s="130"/>
+      <c r="AF36" s="130"/>
+      <c r="AG36" s="130"/>
+      <c r="AH36" s="130"/>
+      <c r="AI36" s="130"/>
+      <c r="AJ36" s="130"/>
+      <c r="AK36" s="130"/>
+      <c r="AL36" s="130"/>
+      <c r="AM36" s="130"/>
+      <c r="AN36" s="130"/>
+      <c r="AO36" s="130"/>
+      <c r="AP36" s="130"/>
+      <c r="AQ36" s="130"/>
+      <c r="AR36" s="130"/>
+      <c r="AS36" s="130"/>
+      <c r="AT36" s="130"/>
+      <c r="AU36" s="130"/>
+      <c r="AV36" s="130"/>
+      <c r="AW36" s="130"/>
+      <c r="AX36" s="130"/>
+      <c r="AY36" s="130"/>
+      <c r="AZ36" s="130"/>
+      <c r="BA36" s="130"/>
+      <c r="BB36" s="130"/>
+      <c r="BC36" s="130"/>
+      <c r="BD36" s="130"/>
+      <c r="BE36" s="130"/>
+      <c r="BF36" s="130"/>
+      <c r="BG36" s="130"/>
+      <c r="BH36" s="130"/>
+      <c r="BI36" s="130"/>
+      <c r="BJ36" s="130"/>
+      <c r="BK36" s="130"/>
+      <c r="BL36" s="130"/>
+      <c r="BM36" s="130"/>
+      <c r="BN36" s="130"/>
+      <c r="BO36" s="130"/>
+      <c r="BP36" s="130"/>
     </row>
     <row r="42" spans="2:68" ht="19.2" x14ac:dyDescent="0.35">
       <c r="C42" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B36:BP36"/>
+    <mergeCell ref="X8:AB8"/>
+    <mergeCell ref="AC8:AG8"/>
+    <mergeCell ref="AH8:AL8"/>
     <mergeCell ref="X7:AL7"/>
     <mergeCell ref="AM7:BA7"/>
     <mergeCell ref="I7:W7"/>
@@ -4476,10 +4483,6 @@
     <mergeCell ref="I8:M8"/>
     <mergeCell ref="N8:R8"/>
     <mergeCell ref="AM8:AQ8"/>
-    <mergeCell ref="B36:BP36"/>
-    <mergeCell ref="X8:AB8"/>
-    <mergeCell ref="AC8:AG8"/>
-    <mergeCell ref="AH8:AL8"/>
   </mergeCells>
   <conditionalFormatting sqref="H10:H34">
     <cfRule type="dataBar" priority="2">
@@ -4537,7 +4540,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O16" sqref="O16"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4602,74 +4605,74 @@
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="114" t="s">
+      <c r="J5" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="115"/>
-      <c r="Q5" s="115"/>
-      <c r="R5" s="115"/>
-      <c r="S5" s="115"/>
-      <c r="T5" s="115"/>
-      <c r="U5" s="115"/>
-      <c r="V5" s="115"/>
-      <c r="W5" s="115"/>
-      <c r="X5" s="116"/>
-      <c r="Y5" s="108" t="s">
+      <c r="K5" s="116"/>
+      <c r="L5" s="116"/>
+      <c r="M5" s="116"/>
+      <c r="N5" s="116"/>
+      <c r="O5" s="116"/>
+      <c r="P5" s="116"/>
+      <c r="Q5" s="116"/>
+      <c r="R5" s="116"/>
+      <c r="S5" s="116"/>
+      <c r="T5" s="116"/>
+      <c r="U5" s="116"/>
+      <c r="V5" s="116"/>
+      <c r="W5" s="116"/>
+      <c r="X5" s="117"/>
+      <c r="Y5" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="Z5" s="109"/>
-      <c r="AA5" s="109"/>
-      <c r="AB5" s="109"/>
-      <c r="AC5" s="109"/>
-      <c r="AD5" s="109"/>
-      <c r="AE5" s="109"/>
-      <c r="AF5" s="109"/>
-      <c r="AG5" s="109"/>
-      <c r="AH5" s="109"/>
-      <c r="AI5" s="109"/>
-      <c r="AJ5" s="109"/>
-      <c r="AK5" s="109"/>
-      <c r="AL5" s="109"/>
-      <c r="AM5" s="110"/>
-      <c r="AN5" s="111" t="s">
+      <c r="Z5" s="110"/>
+      <c r="AA5" s="110"/>
+      <c r="AB5" s="110"/>
+      <c r="AC5" s="110"/>
+      <c r="AD5" s="110"/>
+      <c r="AE5" s="110"/>
+      <c r="AF5" s="110"/>
+      <c r="AG5" s="110"/>
+      <c r="AH5" s="110"/>
+      <c r="AI5" s="110"/>
+      <c r="AJ5" s="110"/>
+      <c r="AK5" s="110"/>
+      <c r="AL5" s="110"/>
+      <c r="AM5" s="111"/>
+      <c r="AN5" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="AO5" s="112"/>
-      <c r="AP5" s="112"/>
-      <c r="AQ5" s="112"/>
-      <c r="AR5" s="112"/>
-      <c r="AS5" s="112"/>
-      <c r="AT5" s="112"/>
-      <c r="AU5" s="112"/>
-      <c r="AV5" s="112"/>
-      <c r="AW5" s="112"/>
-      <c r="AX5" s="112"/>
-      <c r="AY5" s="112"/>
-      <c r="AZ5" s="112"/>
-      <c r="BA5" s="112"/>
-      <c r="BB5" s="113"/>
-      <c r="BC5" s="117" t="s">
+      <c r="AO5" s="113"/>
+      <c r="AP5" s="113"/>
+      <c r="AQ5" s="113"/>
+      <c r="AR5" s="113"/>
+      <c r="AS5" s="113"/>
+      <c r="AT5" s="113"/>
+      <c r="AU5" s="113"/>
+      <c r="AV5" s="113"/>
+      <c r="AW5" s="113"/>
+      <c r="AX5" s="113"/>
+      <c r="AY5" s="113"/>
+      <c r="AZ5" s="113"/>
+      <c r="BA5" s="113"/>
+      <c r="BB5" s="114"/>
+      <c r="BC5" s="118" t="s">
         <v>4</v>
       </c>
-      <c r="BD5" s="118"/>
-      <c r="BE5" s="118"/>
-      <c r="BF5" s="118"/>
-      <c r="BG5" s="118"/>
-      <c r="BH5" s="118"/>
-      <c r="BI5" s="118"/>
-      <c r="BJ5" s="118"/>
-      <c r="BK5" s="118"/>
-      <c r="BL5" s="118"/>
-      <c r="BM5" s="118"/>
-      <c r="BN5" s="118"/>
-      <c r="BO5" s="118"/>
-      <c r="BP5" s="118"/>
-      <c r="BQ5" s="119"/>
+      <c r="BD5" s="119"/>
+      <c r="BE5" s="119"/>
+      <c r="BF5" s="119"/>
+      <c r="BG5" s="119"/>
+      <c r="BH5" s="119"/>
+      <c r="BI5" s="119"/>
+      <c r="BJ5" s="119"/>
+      <c r="BK5" s="119"/>
+      <c r="BL5" s="119"/>
+      <c r="BM5" s="119"/>
+      <c r="BN5" s="119"/>
+      <c r="BO5" s="119"/>
+      <c r="BP5" s="119"/>
+      <c r="BQ5" s="120"/>
     </row>
     <row r="6" spans="2:69" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
@@ -4684,7 +4687,7 @@
       <c r="E6" s="95" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="127" t="s">
+      <c r="F6" s="102" t="s">
         <v>89</v>
       </c>
       <c r="G6" s="96" t="s">
@@ -4696,90 +4699,90 @@
       <c r="I6" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="126" t="s">
+      <c r="J6" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="124"/>
-      <c r="L6" s="124"/>
-      <c r="M6" s="124"/>
-      <c r="N6" s="124"/>
-      <c r="O6" s="124" t="s">
+      <c r="K6" s="126"/>
+      <c r="L6" s="126"/>
+      <c r="M6" s="126"/>
+      <c r="N6" s="126"/>
+      <c r="O6" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="P6" s="124"/>
-      <c r="Q6" s="124"/>
-      <c r="R6" s="124"/>
-      <c r="S6" s="124"/>
-      <c r="T6" s="124" t="s">
+      <c r="P6" s="126"/>
+      <c r="Q6" s="126"/>
+      <c r="R6" s="126"/>
+      <c r="S6" s="126"/>
+      <c r="T6" s="126" t="s">
         <v>7</v>
       </c>
-      <c r="U6" s="124"/>
-      <c r="V6" s="124"/>
-      <c r="W6" s="124"/>
-      <c r="X6" s="125"/>
-      <c r="Y6" s="105" t="s">
+      <c r="U6" s="126"/>
+      <c r="V6" s="126"/>
+      <c r="W6" s="126"/>
+      <c r="X6" s="127"/>
+      <c r="Y6" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="Z6" s="106"/>
-      <c r="AA6" s="106"/>
-      <c r="AB6" s="106"/>
-      <c r="AC6" s="106"/>
-      <c r="AD6" s="106" t="s">
+      <c r="Z6" s="132"/>
+      <c r="AA6" s="132"/>
+      <c r="AB6" s="132"/>
+      <c r="AC6" s="132"/>
+      <c r="AD6" s="132" t="s">
         <v>9</v>
       </c>
-      <c r="AE6" s="106"/>
-      <c r="AF6" s="106"/>
-      <c r="AG6" s="106"/>
-      <c r="AH6" s="106"/>
-      <c r="AI6" s="106" t="s">
+      <c r="AE6" s="132"/>
+      <c r="AF6" s="132"/>
+      <c r="AG6" s="132"/>
+      <c r="AH6" s="132"/>
+      <c r="AI6" s="132" t="s">
         <v>10</v>
       </c>
-      <c r="AJ6" s="106"/>
-      <c r="AK6" s="106"/>
-      <c r="AL6" s="106"/>
-      <c r="AM6" s="107"/>
-      <c r="AN6" s="102" t="s">
+      <c r="AJ6" s="132"/>
+      <c r="AK6" s="132"/>
+      <c r="AL6" s="132"/>
+      <c r="AM6" s="133"/>
+      <c r="AN6" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="AO6" s="103"/>
-      <c r="AP6" s="103"/>
-      <c r="AQ6" s="103"/>
-      <c r="AR6" s="103"/>
-      <c r="AS6" s="103" t="s">
+      <c r="AO6" s="121"/>
+      <c r="AP6" s="121"/>
+      <c r="AQ6" s="121"/>
+      <c r="AR6" s="121"/>
+      <c r="AS6" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="AT6" s="103"/>
-      <c r="AU6" s="103"/>
-      <c r="AV6" s="103"/>
-      <c r="AW6" s="103"/>
-      <c r="AX6" s="103" t="s">
+      <c r="AT6" s="121"/>
+      <c r="AU6" s="121"/>
+      <c r="AV6" s="121"/>
+      <c r="AW6" s="121"/>
+      <c r="AX6" s="121" t="s">
         <v>13</v>
       </c>
-      <c r="AY6" s="103"/>
-      <c r="AZ6" s="103"/>
-      <c r="BA6" s="103"/>
-      <c r="BB6" s="120"/>
-      <c r="BC6" s="121" t="s">
+      <c r="AY6" s="121"/>
+      <c r="AZ6" s="121"/>
+      <c r="BA6" s="121"/>
+      <c r="BB6" s="122"/>
+      <c r="BC6" s="123" t="s">
         <v>14</v>
       </c>
-      <c r="BD6" s="122"/>
-      <c r="BE6" s="122"/>
-      <c r="BF6" s="122"/>
-      <c r="BG6" s="122"/>
-      <c r="BH6" s="122" t="s">
+      <c r="BD6" s="124"/>
+      <c r="BE6" s="124"/>
+      <c r="BF6" s="124"/>
+      <c r="BG6" s="124"/>
+      <c r="BH6" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="BI6" s="122"/>
-      <c r="BJ6" s="122"/>
-      <c r="BK6" s="122"/>
-      <c r="BL6" s="122"/>
-      <c r="BM6" s="122" t="s">
+      <c r="BI6" s="124"/>
+      <c r="BJ6" s="124"/>
+      <c r="BK6" s="124"/>
+      <c r="BL6" s="124"/>
+      <c r="BM6" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="BN6" s="122"/>
-      <c r="BO6" s="122"/>
-      <c r="BP6" s="122"/>
-      <c r="BQ6" s="123"/>
+      <c r="BN6" s="124"/>
+      <c r="BO6" s="124"/>
+      <c r="BP6" s="124"/>
+      <c r="BQ6" s="125"/>
     </row>
     <row r="7" spans="2:69" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="9" t="s">
@@ -4794,7 +4797,7 @@
       <c r="E7" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="128" t="s">
+      <c r="F7" s="103" t="s">
         <v>88</v>
       </c>
       <c r="G7" s="98" t="s">
@@ -5000,7 +5003,7 @@
       <c r="E8" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="129" t="s">
+      <c r="F8" s="104" t="s">
         <v>82</v>
       </c>
       <c r="G8" s="85" t="s">
@@ -5086,7 +5089,7 @@
       <c r="E9" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="129" t="s">
+      <c r="F9" s="104" t="s">
         <v>82</v>
       </c>
       <c r="G9" s="85" t="s">
@@ -5172,7 +5175,7 @@
       <c r="E10" s="87" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="129" t="s">
+      <c r="F10" s="104" t="s">
         <v>82</v>
       </c>
       <c r="G10" s="85" t="s">
@@ -5258,23 +5261,25 @@
       <c r="E11" s="88">
         <v>43892</v>
       </c>
-      <c r="F11" s="130">
+      <c r="F11" s="105">
         <v>43923</v>
       </c>
-      <c r="G11" s="91"/>
+      <c r="G11" s="105">
+        <v>43923</v>
+      </c>
       <c r="H11" s="93">
         <v>1</v>
       </c>
       <c r="I11" s="70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="65"/>
       <c r="K11" s="26"/>
       <c r="L11" s="26"/>
       <c r="M11" s="26"/>
       <c r="N11" s="26"/>
-      <c r="O11" s="133"/>
-      <c r="P11" s="27"/>
+      <c r="O11" s="108"/>
+      <c r="P11" s="108"/>
       <c r="Q11" s="27"/>
       <c r="R11" s="27"/>
       <c r="S11" s="27"/>
@@ -5342,23 +5347,25 @@
       <c r="E12" s="88">
         <v>43892</v>
       </c>
-      <c r="F12" s="130">
+      <c r="F12" s="105">
         <v>43923</v>
       </c>
-      <c r="G12" s="91"/>
+      <c r="G12" s="105">
+        <v>43923</v>
+      </c>
       <c r="H12" s="93">
         <v>1</v>
       </c>
       <c r="I12" s="70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="65"/>
       <c r="K12" s="26"/>
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="26"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
+      <c r="O12" s="101"/>
+      <c r="P12" s="101"/>
       <c r="Q12" s="27"/>
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
@@ -5426,15 +5433,17 @@
       <c r="E13" s="88">
         <v>43923</v>
       </c>
-      <c r="F13" s="130">
+      <c r="F13" s="105">
         <v>43953</v>
       </c>
-      <c r="G13" s="91"/>
+      <c r="G13" s="105">
+        <v>43953</v>
+      </c>
       <c r="H13" s="93">
         <v>1</v>
       </c>
       <c r="I13" s="70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="65"/>
       <c r="K13" s="26"/>
@@ -5442,8 +5451,8 @@
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
       <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
+      <c r="P13" s="101"/>
+      <c r="Q13" s="101"/>
       <c r="R13" s="27"/>
       <c r="S13" s="27"/>
       <c r="T13" s="26"/>
@@ -5510,15 +5519,17 @@
       <c r="E14" s="88">
         <v>43923</v>
       </c>
-      <c r="F14" s="130">
+      <c r="F14" s="105">
         <v>43953</v>
       </c>
-      <c r="G14" s="91"/>
+      <c r="G14" s="105">
+        <v>43953</v>
+      </c>
       <c r="H14" s="93">
         <v>1</v>
       </c>
       <c r="I14" s="70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="65"/>
       <c r="K14" s="26"/>
@@ -5526,8 +5537,8 @@
       <c r="M14" s="26"/>
       <c r="N14" s="26"/>
       <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
+      <c r="P14" s="101"/>
+      <c r="Q14" s="101"/>
       <c r="R14" s="27"/>
       <c r="S14" s="27"/>
       <c r="T14" s="26"/>
@@ -5594,15 +5605,17 @@
       <c r="E15" s="88">
         <v>43953</v>
       </c>
-      <c r="F15" s="130">
+      <c r="F15" s="105">
         <v>44014</v>
       </c>
-      <c r="G15" s="91"/>
+      <c r="G15" s="105">
+        <v>44014</v>
+      </c>
       <c r="H15" s="93">
         <v>2</v>
       </c>
       <c r="I15" s="70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="65"/>
       <c r="K15" s="26"/>
@@ -5611,9 +5624,9 @@
       <c r="N15" s="26"/>
       <c r="O15" s="27"/>
       <c r="P15" s="27"/>
-      <c r="Q15" s="27"/>
-      <c r="R15" s="27"/>
-      <c r="S15" s="27"/>
+      <c r="Q15" s="101"/>
+      <c r="R15" s="101"/>
+      <c r="S15" s="101"/>
       <c r="T15" s="26"/>
       <c r="U15" s="26"/>
       <c r="V15" s="26"/>
@@ -5669,7 +5682,7 @@
       <c r="B16" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="C16" s="134" t="s">
         <v>102</v>
       </c>
       <c r="D16" s="59" t="s">
@@ -5678,15 +5691,17 @@
       <c r="E16" s="89">
         <v>44014</v>
       </c>
-      <c r="F16" s="131">
+      <c r="F16" s="106">
         <v>44045</v>
       </c>
-      <c r="G16" s="86"/>
+      <c r="G16" s="106">
+        <v>44045</v>
+      </c>
       <c r="H16" s="60">
         <v>1</v>
       </c>
       <c r="I16" s="71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="64"/>
       <c r="K16" s="22"/>
@@ -5697,7 +5712,7 @@
       <c r="P16" s="22"/>
       <c r="Q16" s="22"/>
       <c r="R16" s="22"/>
-      <c r="S16" s="22"/>
+      <c r="S16" s="101"/>
       <c r="T16" s="22"/>
       <c r="U16" s="22"/>
       <c r="V16" s="22"/>
@@ -5754,7 +5769,7 @@
       <c r="C17" s="54"/>
       <c r="D17" s="55"/>
       <c r="E17" s="88"/>
-      <c r="F17" s="130"/>
+      <c r="F17" s="105"/>
       <c r="G17" s="91"/>
       <c r="H17" s="93"/>
       <c r="I17" s="70"/>
@@ -5824,7 +5839,7 @@
       <c r="C18" s="54"/>
       <c r="D18" s="55"/>
       <c r="E18" s="88"/>
-      <c r="F18" s="130"/>
+      <c r="F18" s="105"/>
       <c r="G18" s="91"/>
       <c r="H18" s="93"/>
       <c r="I18" s="70"/>
@@ -5894,7 +5909,7 @@
       <c r="C19" s="54"/>
       <c r="D19" s="55"/>
       <c r="E19" s="88"/>
-      <c r="F19" s="130"/>
+      <c r="F19" s="105"/>
       <c r="G19" s="91"/>
       <c r="H19" s="93"/>
       <c r="I19" s="70"/>
@@ -5964,7 +5979,7 @@
       <c r="C20" s="54"/>
       <c r="D20" s="55"/>
       <c r="E20" s="88"/>
-      <c r="F20" s="130"/>
+      <c r="F20" s="105"/>
       <c r="G20" s="91"/>
       <c r="H20" s="93"/>
       <c r="I20" s="70"/>
@@ -6034,7 +6049,7 @@
       <c r="C21" s="58"/>
       <c r="D21" s="59"/>
       <c r="E21" s="89"/>
-      <c r="F21" s="131"/>
+      <c r="F21" s="106"/>
       <c r="G21" s="86"/>
       <c r="H21" s="60"/>
       <c r="I21" s="71"/>
@@ -6104,7 +6119,7 @@
       <c r="C22" s="54"/>
       <c r="D22" s="55"/>
       <c r="E22" s="88"/>
-      <c r="F22" s="130"/>
+      <c r="F22" s="105"/>
       <c r="G22" s="91"/>
       <c r="H22" s="93"/>
       <c r="I22" s="70"/>
@@ -6174,7 +6189,7 @@
       <c r="C23" s="54"/>
       <c r="D23" s="55"/>
       <c r="E23" s="88"/>
-      <c r="F23" s="130"/>
+      <c r="F23" s="105"/>
       <c r="G23" s="91"/>
       <c r="H23" s="93"/>
       <c r="I23" s="70"/>
@@ -6244,7 +6259,7 @@
       <c r="C24" s="56"/>
       <c r="D24" s="57"/>
       <c r="E24" s="88"/>
-      <c r="F24" s="130"/>
+      <c r="F24" s="105"/>
       <c r="G24" s="91"/>
       <c r="H24" s="93"/>
       <c r="I24" s="70"/>
@@ -6314,7 +6329,7 @@
       <c r="C25" s="56"/>
       <c r="D25" s="57"/>
       <c r="E25" s="88"/>
-      <c r="F25" s="130"/>
+      <c r="F25" s="105"/>
       <c r="G25" s="91"/>
       <c r="H25" s="93"/>
       <c r="I25" s="70"/>
@@ -6386,7 +6401,7 @@
       <c r="C26" s="54"/>
       <c r="D26" s="55"/>
       <c r="E26" s="88"/>
-      <c r="F26" s="130"/>
+      <c r="F26" s="105"/>
       <c r="G26" s="91"/>
       <c r="H26" s="93"/>
       <c r="I26" s="70"/>
@@ -6456,7 +6471,7 @@
       <c r="C27" s="56"/>
       <c r="D27" s="57"/>
       <c r="E27" s="88"/>
-      <c r="F27" s="130"/>
+      <c r="F27" s="105"/>
       <c r="G27" s="91"/>
       <c r="H27" s="93"/>
       <c r="I27" s="70"/>
@@ -6526,7 +6541,7 @@
       <c r="C28" s="58"/>
       <c r="D28" s="59"/>
       <c r="E28" s="89"/>
-      <c r="F28" s="131"/>
+      <c r="F28" s="106"/>
       <c r="G28" s="86"/>
       <c r="H28" s="60"/>
       <c r="I28" s="71"/>
@@ -6596,7 +6611,7 @@
       <c r="C29" s="54"/>
       <c r="D29" s="55"/>
       <c r="E29" s="88"/>
-      <c r="F29" s="130"/>
+      <c r="F29" s="105"/>
       <c r="G29" s="91"/>
       <c r="H29" s="93"/>
       <c r="I29" s="70"/>
@@ -6666,7 +6681,7 @@
       <c r="C30" s="54"/>
       <c r="D30" s="55"/>
       <c r="E30" s="88"/>
-      <c r="F30" s="130"/>
+      <c r="F30" s="105"/>
       <c r="G30" s="91"/>
       <c r="H30" s="93"/>
       <c r="I30" s="70"/>
@@ -6736,7 +6751,7 @@
       <c r="C31" s="54"/>
       <c r="D31" s="55"/>
       <c r="E31" s="88"/>
-      <c r="F31" s="130"/>
+      <c r="F31" s="105"/>
       <c r="G31" s="91"/>
       <c r="H31" s="93"/>
       <c r="I31" s="70"/>
@@ -6806,7 +6821,7 @@
       <c r="C32" s="62"/>
       <c r="D32" s="63"/>
       <c r="E32" s="90"/>
-      <c r="F32" s="132"/>
+      <c r="F32" s="107"/>
       <c r="G32" s="92"/>
       <c r="H32" s="94"/>
       <c r="I32" s="72"/>

</xml_diff>

<commit_message>
updating Project plan and RTM
Signed-off-by: NorhanNassar <norhan.nassar96@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PP.xlsx
+++ b/SW deliveries log/PP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16296" yWindow="0" windowWidth="21504" windowHeight="9780" tabRatio="500"/>
+    <workbookView xWindow="18564" yWindow="0" windowWidth="21504" windowHeight="9780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Gantt Chart - BLANK" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="82">
   <si>
     <t>DURATION</t>
   </si>
@@ -1303,7 +1303,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1583,78 +1583,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1682,9 +1610,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="9" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1714,6 +1639,78 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1942,9 +1939,9 @@
   </sheetPr>
   <dimension ref="B1:BR39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z19" sqref="Z19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2014,74 +2011,74 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="121" t="s">
+      <c r="K5" s="140" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="122"/>
-      <c r="M5" s="122"/>
-      <c r="N5" s="122"/>
-      <c r="O5" s="122"/>
-      <c r="P5" s="122"/>
-      <c r="Q5" s="122"/>
-      <c r="R5" s="122"/>
-      <c r="S5" s="122"/>
-      <c r="T5" s="122"/>
-      <c r="U5" s="122"/>
-      <c r="V5" s="122"/>
-      <c r="W5" s="122"/>
-      <c r="X5" s="122"/>
-      <c r="Y5" s="123"/>
-      <c r="Z5" s="124" t="s">
+      <c r="L5" s="141"/>
+      <c r="M5" s="141"/>
+      <c r="N5" s="141"/>
+      <c r="O5" s="141"/>
+      <c r="P5" s="141"/>
+      <c r="Q5" s="141"/>
+      <c r="R5" s="141"/>
+      <c r="S5" s="141"/>
+      <c r="T5" s="141"/>
+      <c r="U5" s="141"/>
+      <c r="V5" s="141"/>
+      <c r="W5" s="141"/>
+      <c r="X5" s="141"/>
+      <c r="Y5" s="142"/>
+      <c r="Z5" s="143" t="s">
         <v>2</v>
       </c>
-      <c r="AA5" s="125"/>
-      <c r="AB5" s="125"/>
-      <c r="AC5" s="125"/>
-      <c r="AD5" s="125"/>
-      <c r="AE5" s="125"/>
-      <c r="AF5" s="125"/>
-      <c r="AG5" s="125"/>
-      <c r="AH5" s="125"/>
-      <c r="AI5" s="125"/>
-      <c r="AJ5" s="125"/>
-      <c r="AK5" s="125"/>
-      <c r="AL5" s="125"/>
-      <c r="AM5" s="125"/>
-      <c r="AN5" s="126"/>
-      <c r="AO5" s="127" t="s">
+      <c r="AA5" s="144"/>
+      <c r="AB5" s="144"/>
+      <c r="AC5" s="144"/>
+      <c r="AD5" s="144"/>
+      <c r="AE5" s="144"/>
+      <c r="AF5" s="144"/>
+      <c r="AG5" s="144"/>
+      <c r="AH5" s="144"/>
+      <c r="AI5" s="144"/>
+      <c r="AJ5" s="144"/>
+      <c r="AK5" s="144"/>
+      <c r="AL5" s="144"/>
+      <c r="AM5" s="144"/>
+      <c r="AN5" s="145"/>
+      <c r="AO5" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="AP5" s="128"/>
-      <c r="AQ5" s="128"/>
-      <c r="AR5" s="128"/>
-      <c r="AS5" s="128"/>
-      <c r="AT5" s="128"/>
-      <c r="AU5" s="128"/>
-      <c r="AV5" s="128"/>
-      <c r="AW5" s="128"/>
-      <c r="AX5" s="128"/>
-      <c r="AY5" s="128"/>
-      <c r="AZ5" s="128"/>
-      <c r="BA5" s="128"/>
-      <c r="BB5" s="128"/>
-      <c r="BC5" s="129"/>
-      <c r="BD5" s="130" t="s">
+      <c r="AP5" s="147"/>
+      <c r="AQ5" s="147"/>
+      <c r="AR5" s="147"/>
+      <c r="AS5" s="147"/>
+      <c r="AT5" s="147"/>
+      <c r="AU5" s="147"/>
+      <c r="AV5" s="147"/>
+      <c r="AW5" s="147"/>
+      <c r="AX5" s="147"/>
+      <c r="AY5" s="147"/>
+      <c r="AZ5" s="147"/>
+      <c r="BA5" s="147"/>
+      <c r="BB5" s="147"/>
+      <c r="BC5" s="148"/>
+      <c r="BD5" s="149" t="s">
         <v>4</v>
       </c>
-      <c r="BE5" s="131"/>
-      <c r="BF5" s="131"/>
-      <c r="BG5" s="131"/>
-      <c r="BH5" s="131"/>
-      <c r="BI5" s="131"/>
-      <c r="BJ5" s="131"/>
-      <c r="BK5" s="131"/>
-      <c r="BL5" s="131"/>
-      <c r="BM5" s="131"/>
-      <c r="BN5" s="131"/>
-      <c r="BO5" s="131"/>
-      <c r="BP5" s="131"/>
-      <c r="BQ5" s="131"/>
-      <c r="BR5" s="132"/>
+      <c r="BE5" s="150"/>
+      <c r="BF5" s="150"/>
+      <c r="BG5" s="150"/>
+      <c r="BH5" s="150"/>
+      <c r="BI5" s="150"/>
+      <c r="BJ5" s="150"/>
+      <c r="BK5" s="150"/>
+      <c r="BL5" s="150"/>
+      <c r="BM5" s="150"/>
+      <c r="BN5" s="150"/>
+      <c r="BO5" s="150"/>
+      <c r="BP5" s="150"/>
+      <c r="BQ5" s="150"/>
+      <c r="BR5" s="151"/>
     </row>
     <row r="6" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
@@ -2111,90 +2108,90 @@
       <c r="J6" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="133" t="s">
+      <c r="K6" s="152" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="134"/>
-      <c r="M6" s="134"/>
-      <c r="N6" s="134"/>
-      <c r="O6" s="134"/>
-      <c r="P6" s="134" t="s">
+      <c r="L6" s="153"/>
+      <c r="M6" s="153"/>
+      <c r="N6" s="153"/>
+      <c r="O6" s="153"/>
+      <c r="P6" s="153" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="134"/>
-      <c r="R6" s="134"/>
-      <c r="S6" s="134"/>
-      <c r="T6" s="134"/>
-      <c r="U6" s="134" t="s">
+      <c r="Q6" s="153"/>
+      <c r="R6" s="153"/>
+      <c r="S6" s="153"/>
+      <c r="T6" s="153"/>
+      <c r="U6" s="153" t="s">
         <v>7</v>
       </c>
-      <c r="V6" s="134"/>
-      <c r="W6" s="134"/>
-      <c r="X6" s="134"/>
-      <c r="Y6" s="135"/>
-      <c r="Z6" s="136" t="s">
+      <c r="V6" s="153"/>
+      <c r="W6" s="153"/>
+      <c r="X6" s="153"/>
+      <c r="Y6" s="154"/>
+      <c r="Z6" s="155" t="s">
         <v>8</v>
       </c>
-      <c r="AA6" s="137"/>
-      <c r="AB6" s="137"/>
-      <c r="AC6" s="137"/>
-      <c r="AD6" s="137"/>
-      <c r="AE6" s="137" t="s">
+      <c r="AA6" s="156"/>
+      <c r="AB6" s="156"/>
+      <c r="AC6" s="156"/>
+      <c r="AD6" s="156"/>
+      <c r="AE6" s="156" t="s">
         <v>9</v>
       </c>
-      <c r="AF6" s="137"/>
-      <c r="AG6" s="137"/>
-      <c r="AH6" s="137"/>
-      <c r="AI6" s="137"/>
-      <c r="AJ6" s="137" t="s">
+      <c r="AF6" s="156"/>
+      <c r="AG6" s="156"/>
+      <c r="AH6" s="156"/>
+      <c r="AI6" s="156"/>
+      <c r="AJ6" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="AK6" s="137"/>
-      <c r="AL6" s="137"/>
-      <c r="AM6" s="137"/>
-      <c r="AN6" s="138"/>
-      <c r="AO6" s="139" t="s">
+      <c r="AK6" s="156"/>
+      <c r="AL6" s="156"/>
+      <c r="AM6" s="156"/>
+      <c r="AN6" s="157"/>
+      <c r="AO6" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="AP6" s="140"/>
-      <c r="AQ6" s="140"/>
-      <c r="AR6" s="140"/>
-      <c r="AS6" s="140"/>
-      <c r="AT6" s="140" t="s">
+      <c r="AP6" s="159"/>
+      <c r="AQ6" s="159"/>
+      <c r="AR6" s="159"/>
+      <c r="AS6" s="159"/>
+      <c r="AT6" s="159" t="s">
         <v>12</v>
       </c>
-      <c r="AU6" s="140"/>
-      <c r="AV6" s="140"/>
-      <c r="AW6" s="140"/>
-      <c r="AX6" s="140"/>
-      <c r="AY6" s="140" t="s">
+      <c r="AU6" s="159"/>
+      <c r="AV6" s="159"/>
+      <c r="AW6" s="159"/>
+      <c r="AX6" s="159"/>
+      <c r="AY6" s="159" t="s">
         <v>13</v>
       </c>
-      <c r="AZ6" s="140"/>
-      <c r="BA6" s="140"/>
-      <c r="BB6" s="140"/>
-      <c r="BC6" s="141"/>
-      <c r="BD6" s="142" t="s">
+      <c r="AZ6" s="159"/>
+      <c r="BA6" s="159"/>
+      <c r="BB6" s="159"/>
+      <c r="BC6" s="160"/>
+      <c r="BD6" s="161" t="s">
         <v>14</v>
       </c>
-      <c r="BE6" s="119"/>
-      <c r="BF6" s="119"/>
-      <c r="BG6" s="119"/>
-      <c r="BH6" s="119"/>
-      <c r="BI6" s="119" t="s">
+      <c r="BE6" s="138"/>
+      <c r="BF6" s="138"/>
+      <c r="BG6" s="138"/>
+      <c r="BH6" s="138"/>
+      <c r="BI6" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="BJ6" s="119"/>
-      <c r="BK6" s="119"/>
-      <c r="BL6" s="119"/>
-      <c r="BM6" s="119"/>
-      <c r="BN6" s="119" t="s">
+      <c r="BJ6" s="138"/>
+      <c r="BK6" s="138"/>
+      <c r="BL6" s="138"/>
+      <c r="BM6" s="138"/>
+      <c r="BN6" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="BO6" s="119"/>
-      <c r="BP6" s="119"/>
-      <c r="BQ6" s="119"/>
-      <c r="BR6" s="120"/>
+      <c r="BO6" s="138"/>
+      <c r="BP6" s="138"/>
+      <c r="BQ6" s="138"/>
+      <c r="BR6" s="139"/>
     </row>
     <row r="7" spans="2:70" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="9" t="s">
@@ -2415,7 +2412,7 @@
       <c r="D8" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="149" t="s">
+      <c r="E8" s="125" t="s">
         <v>43</v>
       </c>
       <c r="F8" s="80" t="s">
@@ -2504,7 +2501,7 @@
       <c r="D9" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="149" t="s">
+      <c r="E9" s="125" t="s">
         <v>44</v>
       </c>
       <c r="F9" s="80" t="s">
@@ -2593,7 +2590,7 @@
       <c r="D10" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="149" t="s">
+      <c r="E10" s="125" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="80" t="s">
@@ -2682,7 +2679,7 @@
       <c r="D11" s="114" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="147" t="s">
+      <c r="E11" s="123" t="s">
         <v>50</v>
       </c>
       <c r="F11" s="81">
@@ -2771,7 +2768,7 @@
       <c r="D12" s="114" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="147" t="s">
+      <c r="E12" s="123" t="s">
         <v>40</v>
       </c>
       <c r="F12" s="81">
@@ -2860,7 +2857,7 @@
       <c r="D13" s="118" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="147" t="s">
+      <c r="E13" s="123" t="s">
         <v>54</v>
       </c>
       <c r="F13" s="81">
@@ -2949,7 +2946,7 @@
       <c r="D14" s="118" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="147" t="s">
+      <c r="E14" s="123" t="s">
         <v>57</v>
       </c>
       <c r="F14" s="81">
@@ -3038,7 +3035,7 @@
       <c r="D15" s="114" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="147" t="s">
+      <c r="E15" s="123" t="s">
         <v>59</v>
       </c>
       <c r="F15" s="81">
@@ -3127,7 +3124,7 @@
       <c r="D16" s="118" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="148" t="s">
+      <c r="E16" s="124" t="s">
         <v>50</v>
       </c>
       <c r="F16" s="99">
@@ -3155,7 +3152,7 @@
       <c r="R16" s="104"/>
       <c r="S16" s="104"/>
       <c r="T16" s="75"/>
-      <c r="U16" s="104"/>
+      <c r="U16" s="75"/>
       <c r="V16" s="104"/>
       <c r="W16" s="104"/>
       <c r="X16" s="104"/>
@@ -3216,7 +3213,7 @@
       <c r="D17" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="147" t="s">
+      <c r="E17" s="123" t="s">
         <v>50</v>
       </c>
       <c r="F17" s="99" t="s">
@@ -3246,11 +3243,11 @@
       <c r="T17" s="27"/>
       <c r="U17" s="26"/>
       <c r="V17" s="26"/>
-      <c r="W17" s="26"/>
-      <c r="X17" s="26"/>
+      <c r="W17" s="75"/>
+      <c r="X17" s="75"/>
       <c r="Y17" s="28"/>
       <c r="Z17" s="25"/>
-      <c r="AA17" s="32"/>
+      <c r="AA17" s="104"/>
       <c r="AB17" s="26"/>
       <c r="AC17" s="26"/>
       <c r="AD17" s="26"/>
@@ -3302,10 +3299,10 @@
       <c r="C18" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="143" t="s">
+      <c r="D18" s="119" t="s">
         <v>77</v>
       </c>
-      <c r="E18" s="147" t="s">
+      <c r="E18" s="123" t="s">
         <v>59</v>
       </c>
       <c r="F18" s="99" t="s">
@@ -3336,8 +3333,8 @@
       <c r="U18" s="26"/>
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
-      <c r="X18" s="26"/>
-      <c r="Y18" s="28"/>
+      <c r="X18" s="75"/>
+      <c r="Y18" s="75"/>
       <c r="Z18" s="25"/>
       <c r="AA18" s="26"/>
       <c r="AB18" s="26"/>
@@ -3385,30 +3382,32 @@
       <c r="BR18" s="31"/>
     </row>
     <row r="19" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="161" t="s">
+      <c r="B19" s="136" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="160" t="s">
+      <c r="C19" s="135" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="144" t="s">
+      <c r="D19" s="120" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="143" t="s">
+      <c r="E19" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="150" t="s">
+      <c r="F19" s="126" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="151" t="s">
+      <c r="G19" s="127" t="s">
         <v>81</v>
       </c>
-      <c r="H19" s="152"/>
-      <c r="I19" s="153">
+      <c r="H19" s="84" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19" s="128">
         <v>1</v>
       </c>
-      <c r="J19" s="154">
-        <v>0</v>
+      <c r="J19" s="129">
+        <v>1</v>
       </c>
       <c r="K19" s="63"/>
       <c r="L19" s="26"/>
@@ -3425,7 +3424,7 @@
       <c r="W19" s="26"/>
       <c r="X19" s="26"/>
       <c r="Y19" s="28"/>
-      <c r="Z19" s="25"/>
+      <c r="Z19" s="32"/>
       <c r="AA19" s="26"/>
       <c r="AB19" s="26"/>
       <c r="AC19" s="26"/>
@@ -3473,16 +3472,16 @@
     </row>
     <row r="20" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="48"/>
-      <c r="C20" s="162"/>
-      <c r="D20" s="145" t="s">
+      <c r="C20" s="137"/>
+      <c r="D20" s="121" t="s">
         <v>79</v>
       </c>
-      <c r="E20" s="146"/>
-      <c r="F20" s="155"/>
-      <c r="G20" s="156"/>
-      <c r="H20" s="157"/>
-      <c r="I20" s="158"/>
-      <c r="J20" s="159"/>
+      <c r="E20" s="122"/>
+      <c r="F20" s="130"/>
+      <c r="G20" s="131"/>
+      <c r="H20" s="132"/>
+      <c r="I20" s="133"/>
+      <c r="J20" s="134"/>
       <c r="K20" s="63"/>
       <c r="L20" s="26"/>
       <c r="M20" s="26"/>

</xml_diff>

<commit_message>
Upload GDD Documentation V0.1
Updating PP

Signed-off-by: NorhanNassar <norhan.nassar96@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PP.xlsx
+++ b/SW deliveries log/PP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20832" yWindow="0" windowWidth="21504" windowHeight="9780" tabRatio="500"/>
+    <workbookView xWindow="25368" yWindow="0" windowWidth="21504" windowHeight="9780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Gantt Chart - BLANK" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="92">
   <si>
     <t>DURATION</t>
   </si>
@@ -277,6 +277,24 @@
   </si>
   <si>
     <t>29/2/2020</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>GDD Documentation</t>
+  </si>
+  <si>
+    <t>Initial Creation for GDD Documentation</t>
+  </si>
+  <si>
+    <t>Cross Review over GDD Documentation</t>
+  </si>
+  <si>
+    <t>GDD Cross Review</t>
+  </si>
+  <si>
+    <t>14</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1333,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1413,9 +1431,6 @@
     <xf numFmtId="49" fontId="5" fillId="9" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1547,9 +1562,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="19" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1577,9 +1589,6 @@
     <xf numFmtId="165" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1628,17 +1637,11 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="9" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1646,6 +1649,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1718,7 +1724,25 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1948,9 +1972,9 @@
   </sheetPr>
   <dimension ref="B1:BR39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomLeft" activeCell="D10" activeCellId="1" sqref="D9 D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1990,22 +2014,22 @@
       <c r="U1" s="47"/>
     </row>
     <row r="2" spans="2:70" s="1" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="111"/>
+      <c r="D2" s="109"/>
     </row>
     <row r="3" spans="2:70" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="112"/>
+      <c r="D3" s="110"/>
     </row>
     <row r="4" spans="2:70" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
@@ -2020,74 +2044,74 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="138" t="s">
+      <c r="K5" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="139"/>
-      <c r="M5" s="139"/>
-      <c r="N5" s="139"/>
-      <c r="O5" s="139"/>
-      <c r="P5" s="139"/>
-      <c r="Q5" s="139"/>
-      <c r="R5" s="139"/>
-      <c r="S5" s="139"/>
-      <c r="T5" s="139"/>
-      <c r="U5" s="139"/>
-      <c r="V5" s="139"/>
-      <c r="W5" s="139"/>
-      <c r="X5" s="139"/>
-      <c r="Y5" s="140"/>
-      <c r="Z5" s="141" t="s">
+      <c r="L5" s="135"/>
+      <c r="M5" s="135"/>
+      <c r="N5" s="135"/>
+      <c r="O5" s="135"/>
+      <c r="P5" s="135"/>
+      <c r="Q5" s="135"/>
+      <c r="R5" s="135"/>
+      <c r="S5" s="135"/>
+      <c r="T5" s="135"/>
+      <c r="U5" s="135"/>
+      <c r="V5" s="135"/>
+      <c r="W5" s="135"/>
+      <c r="X5" s="135"/>
+      <c r="Y5" s="136"/>
+      <c r="Z5" s="137" t="s">
         <v>2</v>
       </c>
-      <c r="AA5" s="142"/>
-      <c r="AB5" s="142"/>
-      <c r="AC5" s="142"/>
-      <c r="AD5" s="142"/>
-      <c r="AE5" s="142"/>
-      <c r="AF5" s="142"/>
-      <c r="AG5" s="142"/>
-      <c r="AH5" s="142"/>
-      <c r="AI5" s="142"/>
-      <c r="AJ5" s="142"/>
-      <c r="AK5" s="142"/>
-      <c r="AL5" s="142"/>
-      <c r="AM5" s="142"/>
-      <c r="AN5" s="143"/>
-      <c r="AO5" s="144" t="s">
+      <c r="AA5" s="138"/>
+      <c r="AB5" s="138"/>
+      <c r="AC5" s="138"/>
+      <c r="AD5" s="138"/>
+      <c r="AE5" s="138"/>
+      <c r="AF5" s="138"/>
+      <c r="AG5" s="138"/>
+      <c r="AH5" s="138"/>
+      <c r="AI5" s="138"/>
+      <c r="AJ5" s="138"/>
+      <c r="AK5" s="138"/>
+      <c r="AL5" s="138"/>
+      <c r="AM5" s="138"/>
+      <c r="AN5" s="139"/>
+      <c r="AO5" s="140" t="s">
         <v>3</v>
       </c>
-      <c r="AP5" s="145"/>
-      <c r="AQ5" s="145"/>
-      <c r="AR5" s="145"/>
-      <c r="AS5" s="145"/>
-      <c r="AT5" s="145"/>
-      <c r="AU5" s="145"/>
-      <c r="AV5" s="145"/>
-      <c r="AW5" s="145"/>
-      <c r="AX5" s="145"/>
-      <c r="AY5" s="145"/>
-      <c r="AZ5" s="145"/>
-      <c r="BA5" s="145"/>
-      <c r="BB5" s="145"/>
-      <c r="BC5" s="146"/>
-      <c r="BD5" s="147" t="s">
+      <c r="AP5" s="141"/>
+      <c r="AQ5" s="141"/>
+      <c r="AR5" s="141"/>
+      <c r="AS5" s="141"/>
+      <c r="AT5" s="141"/>
+      <c r="AU5" s="141"/>
+      <c r="AV5" s="141"/>
+      <c r="AW5" s="141"/>
+      <c r="AX5" s="141"/>
+      <c r="AY5" s="141"/>
+      <c r="AZ5" s="141"/>
+      <c r="BA5" s="141"/>
+      <c r="BB5" s="141"/>
+      <c r="BC5" s="142"/>
+      <c r="BD5" s="143" t="s">
         <v>4</v>
       </c>
-      <c r="BE5" s="148"/>
-      <c r="BF5" s="148"/>
-      <c r="BG5" s="148"/>
-      <c r="BH5" s="148"/>
-      <c r="BI5" s="148"/>
-      <c r="BJ5" s="148"/>
-      <c r="BK5" s="148"/>
-      <c r="BL5" s="148"/>
-      <c r="BM5" s="148"/>
-      <c r="BN5" s="148"/>
-      <c r="BO5" s="148"/>
-      <c r="BP5" s="148"/>
-      <c r="BQ5" s="148"/>
-      <c r="BR5" s="149"/>
+      <c r="BE5" s="144"/>
+      <c r="BF5" s="144"/>
+      <c r="BG5" s="144"/>
+      <c r="BH5" s="144"/>
+      <c r="BI5" s="144"/>
+      <c r="BJ5" s="144"/>
+      <c r="BK5" s="144"/>
+      <c r="BL5" s="144"/>
+      <c r="BM5" s="144"/>
+      <c r="BN5" s="144"/>
+      <c r="BO5" s="144"/>
+      <c r="BP5" s="144"/>
+      <c r="BQ5" s="144"/>
+      <c r="BR5" s="145"/>
     </row>
     <row r="6" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
@@ -2102,105 +2126,105 @@
       <c r="E6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="88" t="s">
+      <c r="F6" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="92" t="s">
+      <c r="G6" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="89" t="s">
+      <c r="H6" s="88" t="s">
         <v>29</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="65" t="s">
+      <c r="J6" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="150" t="s">
+      <c r="K6" s="146" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="151"/>
-      <c r="M6" s="151"/>
-      <c r="N6" s="151"/>
-      <c r="O6" s="151"/>
-      <c r="P6" s="151" t="s">
+      <c r="L6" s="147"/>
+      <c r="M6" s="147"/>
+      <c r="N6" s="147"/>
+      <c r="O6" s="147"/>
+      <c r="P6" s="147" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="151"/>
-      <c r="R6" s="151"/>
-      <c r="S6" s="151"/>
-      <c r="T6" s="151"/>
-      <c r="U6" s="151" t="s">
+      <c r="Q6" s="147"/>
+      <c r="R6" s="147"/>
+      <c r="S6" s="147"/>
+      <c r="T6" s="147"/>
+      <c r="U6" s="147" t="s">
         <v>7</v>
       </c>
-      <c r="V6" s="151"/>
-      <c r="W6" s="151"/>
-      <c r="X6" s="151"/>
-      <c r="Y6" s="152"/>
-      <c r="Z6" s="153" t="s">
+      <c r="V6" s="147"/>
+      <c r="W6" s="147"/>
+      <c r="X6" s="147"/>
+      <c r="Y6" s="148"/>
+      <c r="Z6" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="AA6" s="154"/>
-      <c r="AB6" s="154"/>
-      <c r="AC6" s="154"/>
-      <c r="AD6" s="154"/>
-      <c r="AE6" s="154" t="s">
+      <c r="AA6" s="150"/>
+      <c r="AB6" s="150"/>
+      <c r="AC6" s="150"/>
+      <c r="AD6" s="150"/>
+      <c r="AE6" s="150" t="s">
         <v>9</v>
       </c>
-      <c r="AF6" s="154"/>
-      <c r="AG6" s="154"/>
-      <c r="AH6" s="154"/>
-      <c r="AI6" s="154"/>
-      <c r="AJ6" s="154" t="s">
+      <c r="AF6" s="150"/>
+      <c r="AG6" s="150"/>
+      <c r="AH6" s="150"/>
+      <c r="AI6" s="150"/>
+      <c r="AJ6" s="150" t="s">
         <v>10</v>
       </c>
-      <c r="AK6" s="154"/>
-      <c r="AL6" s="154"/>
-      <c r="AM6" s="154"/>
-      <c r="AN6" s="155"/>
-      <c r="AO6" s="156" t="s">
+      <c r="AK6" s="150"/>
+      <c r="AL6" s="150"/>
+      <c r="AM6" s="150"/>
+      <c r="AN6" s="151"/>
+      <c r="AO6" s="152" t="s">
         <v>11</v>
       </c>
-      <c r="AP6" s="157"/>
-      <c r="AQ6" s="157"/>
-      <c r="AR6" s="157"/>
-      <c r="AS6" s="157"/>
-      <c r="AT6" s="157" t="s">
+      <c r="AP6" s="153"/>
+      <c r="AQ6" s="153"/>
+      <c r="AR6" s="153"/>
+      <c r="AS6" s="153"/>
+      <c r="AT6" s="153" t="s">
         <v>12</v>
       </c>
-      <c r="AU6" s="157"/>
-      <c r="AV6" s="157"/>
-      <c r="AW6" s="157"/>
-      <c r="AX6" s="157"/>
-      <c r="AY6" s="157" t="s">
+      <c r="AU6" s="153"/>
+      <c r="AV6" s="153"/>
+      <c r="AW6" s="153"/>
+      <c r="AX6" s="153"/>
+      <c r="AY6" s="153" t="s">
         <v>13</v>
       </c>
-      <c r="AZ6" s="157"/>
-      <c r="BA6" s="157"/>
-      <c r="BB6" s="157"/>
-      <c r="BC6" s="158"/>
-      <c r="BD6" s="159" t="s">
+      <c r="AZ6" s="153"/>
+      <c r="BA6" s="153"/>
+      <c r="BB6" s="153"/>
+      <c r="BC6" s="154"/>
+      <c r="BD6" s="155" t="s">
         <v>14</v>
       </c>
-      <c r="BE6" s="136"/>
-      <c r="BF6" s="136"/>
-      <c r="BG6" s="136"/>
-      <c r="BH6" s="136"/>
-      <c r="BI6" s="136" t="s">
+      <c r="BE6" s="132"/>
+      <c r="BF6" s="132"/>
+      <c r="BG6" s="132"/>
+      <c r="BH6" s="132"/>
+      <c r="BI6" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="BJ6" s="136"/>
-      <c r="BK6" s="136"/>
-      <c r="BL6" s="136"/>
-      <c r="BM6" s="136"/>
-      <c r="BN6" s="136" t="s">
+      <c r="BJ6" s="132"/>
+      <c r="BK6" s="132"/>
+      <c r="BL6" s="132"/>
+      <c r="BM6" s="132"/>
+      <c r="BN6" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="BO6" s="136"/>
-      <c r="BP6" s="136"/>
-      <c r="BQ6" s="136"/>
-      <c r="BR6" s="137"/>
+      <c r="BO6" s="132"/>
+      <c r="BP6" s="132"/>
+      <c r="BQ6" s="132"/>
+      <c r="BR6" s="133"/>
     </row>
     <row r="7" spans="2:70" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="9" t="s">
@@ -2215,19 +2239,19 @@
       <c r="E7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="90" t="s">
+      <c r="F7" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="93" t="s">
+      <c r="G7" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="91" t="s">
+      <c r="H7" s="90" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="66" t="s">
+      <c r="J7" s="65" t="s">
         <v>30</v>
       </c>
       <c r="K7" s="12" t="s">
@@ -2415,33 +2439,33 @@
       <c r="B8" s="48">
         <v>1</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="158" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="113" t="s">
+      <c r="D8" s="157" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="124" t="s">
+      <c r="E8" s="121" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="94" t="s">
+      <c r="G8" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="78" t="s">
+      <c r="H8" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="I8" s="50">
+      <c r="I8" s="49">
         <v>1</v>
       </c>
-      <c r="J8" s="67">
+      <c r="J8" s="66">
         <v>1</v>
       </c>
-      <c r="K8" s="62"/>
-      <c r="L8" s="75"/>
-      <c r="M8" s="110"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="108"/>
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
       <c r="P8" s="22"/>
@@ -2504,34 +2528,34 @@
       <c r="B9" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="159" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="113" t="s">
+      <c r="D9" s="157" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="124" t="s">
+      <c r="E9" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="80" t="s">
+      <c r="F9" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="94" t="s">
+      <c r="G9" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="78" t="s">
+      <c r="H9" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="50">
+      <c r="I9" s="49">
         <v>1</v>
       </c>
-      <c r="J9" s="67">
+      <c r="J9" s="66">
         <v>1</v>
       </c>
-      <c r="K9" s="62"/>
-      <c r="L9" s="110"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="110"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="108"/>
+      <c r="M9" s="74"/>
+      <c r="N9" s="108"/>
       <c r="O9" s="22"/>
       <c r="P9" s="22"/>
       <c r="Q9" s="22"/>
@@ -2593,34 +2617,34 @@
       <c r="B10" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="158" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="113" t="s">
+      <c r="D10" s="157" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="124" t="s">
+      <c r="E10" s="121" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="80" t="s">
+      <c r="F10" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="94" t="s">
+      <c r="G10" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="78" t="s">
+      <c r="H10" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="I10" s="50">
+      <c r="I10" s="49">
         <v>1</v>
       </c>
-      <c r="J10" s="67">
+      <c r="J10" s="66">
         <v>1</v>
       </c>
-      <c r="K10" s="62"/>
-      <c r="L10" s="110"/>
-      <c r="M10" s="75"/>
-      <c r="N10" s="110"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="108"/>
+      <c r="M10" s="74"/>
+      <c r="N10" s="108"/>
       <c r="O10" s="22"/>
       <c r="P10" s="22"/>
       <c r="Q10" s="22"/>
@@ -2679,40 +2703,40 @@
       <c r="BR10" s="24"/>
     </row>
     <row r="11" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="114" t="s">
+      <c r="D11" s="111" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="122" t="s">
+      <c r="E11" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="81">
+      <c r="F11" s="80">
         <v>43892</v>
       </c>
-      <c r="G11" s="95">
+      <c r="G11" s="94">
         <v>43923</v>
       </c>
-      <c r="H11" s="95">
+      <c r="H11" s="94">
         <v>43923</v>
       </c>
-      <c r="I11" s="86">
+      <c r="I11" s="85">
         <v>1</v>
       </c>
-      <c r="J11" s="68">
+      <c r="J11" s="67">
         <v>1</v>
       </c>
-      <c r="K11" s="63"/>
+      <c r="K11" s="62"/>
       <c r="L11" s="26"/>
       <c r="M11" s="26"/>
       <c r="N11" s="26"/>
       <c r="O11" s="26"/>
-      <c r="P11" s="108"/>
-      <c r="Q11" s="109"/>
+      <c r="P11" s="106"/>
+      <c r="Q11" s="107"/>
       <c r="R11" s="27"/>
       <c r="S11" s="27"/>
       <c r="T11" s="27"/>
@@ -2768,40 +2792,40 @@
       <c r="BR11" s="31"/>
     </row>
     <row r="12" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="160" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="114" t="s">
+      <c r="D12" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="122" t="s">
+      <c r="E12" s="119" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="81">
+      <c r="F12" s="80">
         <v>43892</v>
       </c>
-      <c r="G12" s="95">
+      <c r="G12" s="94">
         <v>43923</v>
       </c>
-      <c r="H12" s="95">
+      <c r="H12" s="94">
         <v>43923</v>
       </c>
-      <c r="I12" s="86">
+      <c r="I12" s="85">
         <v>1</v>
       </c>
-      <c r="J12" s="68">
+      <c r="J12" s="67">
         <v>1</v>
       </c>
-      <c r="K12" s="63"/>
+      <c r="K12" s="62"/>
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="26"/>
       <c r="O12" s="26"/>
-      <c r="P12" s="75"/>
-      <c r="Q12" s="104"/>
+      <c r="P12" s="74"/>
+      <c r="Q12" s="102"/>
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
       <c r="T12" s="27"/>
@@ -2857,41 +2881,41 @@
       <c r="BR12" s="31"/>
     </row>
     <row r="13" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="160" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="118" t="s">
+      <c r="D13" s="115" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="122" t="s">
+      <c r="E13" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="81">
+      <c r="F13" s="80">
         <v>43923</v>
       </c>
-      <c r="G13" s="95">
+      <c r="G13" s="94">
         <v>43953</v>
       </c>
-      <c r="H13" s="95">
+      <c r="H13" s="94">
         <v>43953</v>
       </c>
-      <c r="I13" s="86">
+      <c r="I13" s="85">
         <v>1</v>
       </c>
-      <c r="J13" s="68">
+      <c r="J13" s="67">
         <v>1</v>
       </c>
-      <c r="K13" s="63"/>
+      <c r="K13" s="62"/>
       <c r="L13" s="26"/>
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
       <c r="O13" s="26"/>
       <c r="P13" s="27"/>
-      <c r="Q13" s="75"/>
-      <c r="R13" s="104"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="102"/>
       <c r="S13" s="27"/>
       <c r="T13" s="27"/>
       <c r="U13" s="26"/>
@@ -2946,41 +2970,41 @@
       <c r="BR13" s="31"/>
     </row>
     <row r="14" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="160" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="118" t="s">
+      <c r="D14" s="115" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="122" t="s">
+      <c r="E14" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="81">
+      <c r="F14" s="80">
         <v>43923</v>
       </c>
-      <c r="G14" s="95">
+      <c r="G14" s="94">
         <v>43953</v>
       </c>
-      <c r="H14" s="95">
+      <c r="H14" s="94">
         <v>43953</v>
       </c>
-      <c r="I14" s="86">
+      <c r="I14" s="85">
         <v>1</v>
       </c>
-      <c r="J14" s="68">
+      <c r="J14" s="67">
         <v>1</v>
       </c>
-      <c r="K14" s="63"/>
+      <c r="K14" s="62"/>
       <c r="L14" s="26"/>
       <c r="M14" s="26"/>
       <c r="N14" s="26"/>
       <c r="O14" s="26"/>
       <c r="P14" s="27"/>
-      <c r="Q14" s="75"/>
-      <c r="R14" s="104"/>
+      <c r="Q14" s="74"/>
+      <c r="R14" s="102"/>
       <c r="S14" s="27"/>
       <c r="T14" s="27"/>
       <c r="U14" s="26"/>
@@ -3035,43 +3059,43 @@
       <c r="BR14" s="31"/>
     </row>
     <row r="15" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="51" t="s">
+      <c r="B15" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="114" t="s">
+      <c r="D15" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="122" t="s">
+      <c r="E15" s="119" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="81">
+      <c r="F15" s="80">
         <v>43953</v>
       </c>
-      <c r="G15" s="95">
+      <c r="G15" s="94">
         <v>44014</v>
       </c>
-      <c r="H15" s="95">
+      <c r="H15" s="94">
         <v>44014</v>
       </c>
-      <c r="I15" s="86">
+      <c r="I15" s="85">
         <v>2</v>
       </c>
-      <c r="J15" s="68">
+      <c r="J15" s="67">
         <v>1</v>
       </c>
-      <c r="K15" s="63"/>
+      <c r="K15" s="62"/>
       <c r="L15" s="26"/>
       <c r="M15" s="26"/>
       <c r="N15" s="26"/>
       <c r="O15" s="26"/>
       <c r="P15" s="27"/>
       <c r="Q15" s="27"/>
-      <c r="R15" s="75"/>
-      <c r="S15" s="75"/>
-      <c r="T15" s="104"/>
+      <c r="R15" s="74"/>
+      <c r="S15" s="74"/>
+      <c r="T15" s="102"/>
       <c r="U15" s="26"/>
       <c r="V15" s="26"/>
       <c r="W15" s="26"/>
@@ -3124,123 +3148,123 @@
       <c r="BR15" s="31"/>
     </row>
     <row r="16" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="98" t="s">
+      <c r="C16" s="161" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="118" t="s">
+      <c r="D16" s="115" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="123" t="s">
+      <c r="E16" s="120" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="99">
+      <c r="F16" s="97">
         <v>44014</v>
       </c>
-      <c r="G16" s="100">
+      <c r="G16" s="98">
         <v>44045</v>
       </c>
-      <c r="H16" s="100">
+      <c r="H16" s="98">
         <v>44045</v>
       </c>
-      <c r="I16" s="101">
+      <c r="I16" s="99">
         <v>1</v>
       </c>
-      <c r="J16" s="102">
+      <c r="J16" s="100">
         <v>1</v>
       </c>
-      <c r="K16" s="103"/>
-      <c r="L16" s="104"/>
-      <c r="M16" s="104"/>
-      <c r="N16" s="104"/>
-      <c r="O16" s="104"/>
-      <c r="P16" s="104"/>
-      <c r="Q16" s="104"/>
-      <c r="R16" s="104"/>
-      <c r="S16" s="104"/>
-      <c r="T16" s="75"/>
-      <c r="U16" s="75"/>
-      <c r="V16" s="104"/>
-      <c r="W16" s="104"/>
-      <c r="X16" s="104"/>
-      <c r="Y16" s="105"/>
-      <c r="Z16" s="106"/>
-      <c r="AA16" s="104"/>
-      <c r="AB16" s="104"/>
-      <c r="AC16" s="104"/>
-      <c r="AD16" s="104"/>
-      <c r="AE16" s="104"/>
-      <c r="AF16" s="104"/>
-      <c r="AG16" s="104"/>
-      <c r="AH16" s="104"/>
-      <c r="AI16" s="104"/>
-      <c r="AJ16" s="104"/>
-      <c r="AK16" s="104"/>
-      <c r="AL16" s="104"/>
-      <c r="AM16" s="104"/>
-      <c r="AN16" s="105"/>
-      <c r="AO16" s="106"/>
-      <c r="AP16" s="104"/>
-      <c r="AQ16" s="104"/>
-      <c r="AR16" s="104"/>
-      <c r="AS16" s="104"/>
-      <c r="AT16" s="104"/>
-      <c r="AU16" s="104"/>
-      <c r="AV16" s="104"/>
-      <c r="AW16" s="104"/>
-      <c r="AX16" s="104"/>
-      <c r="AY16" s="104"/>
-      <c r="AZ16" s="104"/>
-      <c r="BA16" s="104"/>
-      <c r="BB16" s="104"/>
-      <c r="BC16" s="105"/>
-      <c r="BD16" s="106"/>
-      <c r="BE16" s="104"/>
-      <c r="BF16" s="104"/>
-      <c r="BG16" s="104"/>
-      <c r="BH16" s="104"/>
-      <c r="BI16" s="104"/>
-      <c r="BJ16" s="104"/>
-      <c r="BK16" s="104"/>
-      <c r="BL16" s="104"/>
-      <c r="BM16" s="104"/>
-      <c r="BN16" s="104"/>
-      <c r="BO16" s="104"/>
-      <c r="BP16" s="104"/>
-      <c r="BQ16" s="104"/>
-      <c r="BR16" s="107"/>
+      <c r="K16" s="101"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="102"/>
+      <c r="N16" s="102"/>
+      <c r="O16" s="102"/>
+      <c r="P16" s="102"/>
+      <c r="Q16" s="102"/>
+      <c r="R16" s="102"/>
+      <c r="S16" s="102"/>
+      <c r="T16" s="74"/>
+      <c r="U16" s="74"/>
+      <c r="V16" s="102"/>
+      <c r="W16" s="102"/>
+      <c r="X16" s="102"/>
+      <c r="Y16" s="103"/>
+      <c r="Z16" s="104"/>
+      <c r="AA16" s="102"/>
+      <c r="AB16" s="102"/>
+      <c r="AC16" s="102"/>
+      <c r="AD16" s="102"/>
+      <c r="AE16" s="102"/>
+      <c r="AF16" s="102"/>
+      <c r="AG16" s="102"/>
+      <c r="AH16" s="102"/>
+      <c r="AI16" s="102"/>
+      <c r="AJ16" s="102"/>
+      <c r="AK16" s="102"/>
+      <c r="AL16" s="102"/>
+      <c r="AM16" s="102"/>
+      <c r="AN16" s="103"/>
+      <c r="AO16" s="104"/>
+      <c r="AP16" s="102"/>
+      <c r="AQ16" s="102"/>
+      <c r="AR16" s="102"/>
+      <c r="AS16" s="102"/>
+      <c r="AT16" s="102"/>
+      <c r="AU16" s="102"/>
+      <c r="AV16" s="102"/>
+      <c r="AW16" s="102"/>
+      <c r="AX16" s="102"/>
+      <c r="AY16" s="102"/>
+      <c r="AZ16" s="102"/>
+      <c r="BA16" s="102"/>
+      <c r="BB16" s="102"/>
+      <c r="BC16" s="103"/>
+      <c r="BD16" s="104"/>
+      <c r="BE16" s="102"/>
+      <c r="BF16" s="102"/>
+      <c r="BG16" s="102"/>
+      <c r="BH16" s="102"/>
+      <c r="BI16" s="102"/>
+      <c r="BJ16" s="102"/>
+      <c r="BK16" s="102"/>
+      <c r="BL16" s="102"/>
+      <c r="BM16" s="102"/>
+      <c r="BN16" s="102"/>
+      <c r="BO16" s="102"/>
+      <c r="BP16" s="102"/>
+      <c r="BQ16" s="102"/>
+      <c r="BR16" s="105"/>
     </row>
     <row r="17" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="160" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="114" t="s">
+      <c r="D17" s="111" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="122" t="s">
+      <c r="E17" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="99" t="s">
+      <c r="F17" s="97" t="s">
         <v>70</v>
       </c>
-      <c r="G17" s="100" t="s">
+      <c r="G17" s="98" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="100" t="s">
+      <c r="H17" s="98" t="s">
         <v>69</v>
       </c>
-      <c r="I17" s="86">
+      <c r="I17" s="85">
         <v>1</v>
       </c>
-      <c r="J17" s="68">
+      <c r="J17" s="67">
         <v>1</v>
       </c>
-      <c r="K17" s="63"/>
+      <c r="K17" s="62"/>
       <c r="L17" s="26"/>
       <c r="M17" s="26"/>
       <c r="N17" s="26"/>
@@ -3252,11 +3276,11 @@
       <c r="T17" s="27"/>
       <c r="U17" s="26"/>
       <c r="V17" s="26"/>
-      <c r="W17" s="75"/>
-      <c r="X17" s="75"/>
+      <c r="W17" s="74"/>
+      <c r="X17" s="74"/>
       <c r="Y17" s="28"/>
       <c r="Z17" s="25"/>
-      <c r="AA17" s="104"/>
+      <c r="AA17" s="102"/>
       <c r="AB17" s="26"/>
       <c r="AC17" s="26"/>
       <c r="AD17" s="26"/>
@@ -3302,34 +3326,34 @@
       <c r="BR17" s="31"/>
     </row>
     <row r="18" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="160" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="119" t="s">
+      <c r="D18" s="116" t="s">
         <v>77</v>
       </c>
-      <c r="E18" s="122" t="s">
+      <c r="E18" s="119" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="99" t="s">
+      <c r="F18" s="97" t="s">
         <v>69</v>
       </c>
-      <c r="G18" s="99" t="s">
+      <c r="G18" s="97" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="84" t="s">
+      <c r="H18" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="I18" s="86">
+      <c r="I18" s="85">
         <v>1</v>
       </c>
-      <c r="J18" s="68">
+      <c r="J18" s="67">
         <v>1</v>
       </c>
-      <c r="K18" s="63"/>
+      <c r="K18" s="62"/>
       <c r="L18" s="26"/>
       <c r="M18" s="26"/>
       <c r="N18" s="26"/>
@@ -3342,8 +3366,8 @@
       <c r="U18" s="26"/>
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
-      <c r="X18" s="75"/>
-      <c r="Y18" s="75"/>
+      <c r="X18" s="74"/>
+      <c r="Y18" s="74"/>
       <c r="Z18" s="25"/>
       <c r="AA18" s="26"/>
       <c r="AB18" s="26"/>
@@ -3391,34 +3415,34 @@
       <c r="BR18" s="31"/>
     </row>
     <row r="19" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="134" t="s">
+      <c r="B19" s="129" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="133" t="s">
+      <c r="C19" s="162" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="120" t="s">
+      <c r="D19" s="117" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="119" t="s">
+      <c r="E19" s="116" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="125" t="s">
+      <c r="F19" s="122" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="126" t="s">
+      <c r="G19" s="123" t="s">
         <v>81</v>
       </c>
-      <c r="H19" s="84" t="s">
+      <c r="H19" s="83" t="s">
         <v>69</v>
       </c>
-      <c r="I19" s="127">
+      <c r="I19" s="124">
         <v>1</v>
       </c>
-      <c r="J19" s="128">
+      <c r="J19" s="125">
         <v>1</v>
       </c>
-      <c r="K19" s="63"/>
+      <c r="K19" s="62"/>
       <c r="L19" s="26"/>
       <c r="M19" s="26"/>
       <c r="N19" s="26"/>
@@ -3481,27 +3505,11 @@
     </row>
     <row r="20" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="48"/>
-      <c r="C20" s="135"/>
-      <c r="D20" s="121" t="s">
+      <c r="C20" s="130"/>
+      <c r="D20" s="118" t="s">
         <v>79</v>
       </c>
-      <c r="E20" s="160" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" s="129" t="s">
-        <v>83</v>
-      </c>
-      <c r="G20" s="129" t="s">
-        <v>84</v>
-      </c>
-      <c r="H20" s="130"/>
-      <c r="I20" s="131">
-        <v>1</v>
-      </c>
-      <c r="J20" s="132">
-        <v>0</v>
-      </c>
-      <c r="K20" s="63"/>
+      <c r="K20" s="62"/>
       <c r="L20" s="26"/>
       <c r="M20" s="26"/>
       <c r="N20" s="26"/>
@@ -3563,26 +3571,34 @@
       <c r="BR20" s="31"/>
     </row>
     <row r="21" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="51"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="113"/>
-      <c r="E21" s="119" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="82" t="s">
+      <c r="B21" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="156" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="157" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="131" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="126" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" s="126" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="96" t="s">
-        <v>85</v>
-      </c>
-      <c r="H21" s="79"/>
-      <c r="I21" s="58">
+      <c r="H21" s="126" t="s">
+        <v>84</v>
+      </c>
+      <c r="I21" s="127">
         <v>1</v>
       </c>
-      <c r="J21" s="69">
-        <v>0</v>
-      </c>
-      <c r="K21" s="62"/>
+      <c r="J21" s="128">
+        <v>1</v>
+      </c>
+      <c r="K21" s="61"/>
       <c r="L21" s="22"/>
       <c r="M21" s="22"/>
       <c r="N21" s="22"/>
@@ -3644,16 +3660,32 @@
       <c r="BR21" s="24"/>
     </row>
     <row r="22" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="51"/>
-      <c r="C22" s="52"/>
-      <c r="D22" s="114"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="81"/>
-      <c r="G22" s="95"/>
-      <c r="H22" s="84"/>
-      <c r="I22" s="86"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="63"/>
+      <c r="B22" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="160" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="115" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="116" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="81" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="95" t="s">
+        <v>85</v>
+      </c>
+      <c r="H22" s="83"/>
+      <c r="I22" s="57">
+        <v>1</v>
+      </c>
+      <c r="J22" s="68">
+        <v>0.5</v>
+      </c>
+      <c r="K22" s="62"/>
       <c r="L22" s="26"/>
       <c r="M22" s="26"/>
       <c r="N22" s="26"/>
@@ -3684,7 +3716,7 @@
       <c r="AM22" s="26"/>
       <c r="AN22" s="28"/>
       <c r="AO22" s="25"/>
-      <c r="AP22" s="76"/>
+      <c r="AP22" s="75"/>
       <c r="AQ22" s="26"/>
       <c r="AR22" s="26"/>
       <c r="AS22" s="26"/>
@@ -3715,16 +3747,16 @@
       <c r="BR22" s="31"/>
     </row>
     <row r="23" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="51"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="114"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="95"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="86"/>
-      <c r="J23" s="68"/>
-      <c r="K23" s="63"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="111"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="94"/>
+      <c r="H23" s="83"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="62"/>
       <c r="L23" s="26"/>
       <c r="M23" s="26"/>
       <c r="N23" s="26"/>
@@ -3786,16 +3818,16 @@
       <c r="BR23" s="31"/>
     </row>
     <row r="24" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="51"/>
-      <c r="C24" s="54"/>
-      <c r="D24" s="116"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="95"/>
-      <c r="H24" s="84"/>
-      <c r="I24" s="86"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="63"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="113"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="94"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="62"/>
       <c r="L24" s="26"/>
       <c r="M24" s="26"/>
       <c r="N24" s="26"/>
@@ -3857,16 +3889,16 @@
       <c r="BR24" s="31"/>
     </row>
     <row r="25" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="51"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="116"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="95"/>
-      <c r="H25" s="84"/>
-      <c r="I25" s="86"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="63"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="113"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="94"/>
+      <c r="H25" s="83"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="62"/>
       <c r="L25" s="26"/>
       <c r="M25" s="26"/>
       <c r="N25" s="26"/>
@@ -3930,16 +3962,16 @@
       <c r="BR25" s="31"/>
     </row>
     <row r="26" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="51"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="114"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="95"/>
-      <c r="H26" s="84"/>
-      <c r="I26" s="86"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="63"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="111"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="94"/>
+      <c r="H26" s="83"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="62"/>
       <c r="L26" s="26"/>
       <c r="M26" s="26"/>
       <c r="N26" s="26"/>
@@ -4001,16 +4033,16 @@
       <c r="BR26" s="31"/>
     </row>
     <row r="27" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="51"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="116"/>
-      <c r="E27" s="55"/>
-      <c r="F27" s="81"/>
-      <c r="G27" s="95"/>
-      <c r="H27" s="84"/>
-      <c r="I27" s="86"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="63"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="113"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="80"/>
+      <c r="G27" s="94"/>
+      <c r="H27" s="83"/>
+      <c r="I27" s="85"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="62"/>
       <c r="L27" s="26"/>
       <c r="M27" s="26"/>
       <c r="N27" s="26"/>
@@ -4072,16 +4104,16 @@
       <c r="BR27" s="31"/>
     </row>
     <row r="28" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="51"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="115"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="82"/>
-      <c r="G28" s="96"/>
-      <c r="H28" s="79"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="62"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="81"/>
+      <c r="G28" s="95"/>
+      <c r="H28" s="78"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="61"/>
       <c r="L28" s="22"/>
       <c r="M28" s="22"/>
       <c r="N28" s="22"/>
@@ -4143,16 +4175,16 @@
       <c r="BR28" s="24"/>
     </row>
     <row r="29" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="51"/>
-      <c r="C29" s="52"/>
-      <c r="D29" s="114"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="81"/>
-      <c r="G29" s="95"/>
-      <c r="H29" s="84"/>
-      <c r="I29" s="86"/>
-      <c r="J29" s="68"/>
-      <c r="K29" s="63"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="111"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="80"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="83"/>
+      <c r="I29" s="85"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="62"/>
       <c r="L29" s="26"/>
       <c r="M29" s="26"/>
       <c r="N29" s="26"/>
@@ -4198,7 +4230,7 @@
       <c r="BB29" s="26"/>
       <c r="BC29" s="28"/>
       <c r="BD29" s="25"/>
-      <c r="BE29" s="77"/>
+      <c r="BE29" s="76"/>
       <c r="BF29" s="26"/>
       <c r="BG29" s="26"/>
       <c r="BH29" s="26"/>
@@ -4214,16 +4246,16 @@
       <c r="BR29" s="31"/>
     </row>
     <row r="30" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="51"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="114"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="81"/>
-      <c r="G30" s="95"/>
-      <c r="H30" s="84"/>
-      <c r="I30" s="86"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="63"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="111"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="80"/>
+      <c r="G30" s="94"/>
+      <c r="H30" s="83"/>
+      <c r="I30" s="85"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="62"/>
       <c r="L30" s="26"/>
       <c r="M30" s="26"/>
       <c r="N30" s="26"/>
@@ -4285,16 +4317,16 @@
       <c r="BR30" s="31"/>
     </row>
     <row r="31" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="51"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="114"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="81"/>
-      <c r="G31" s="95"/>
-      <c r="H31" s="84"/>
-      <c r="I31" s="86"/>
-      <c r="J31" s="68"/>
-      <c r="K31" s="63"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="111"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="94"/>
+      <c r="H31" s="83"/>
+      <c r="I31" s="85"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="62"/>
       <c r="L31" s="26"/>
       <c r="M31" s="26"/>
       <c r="N31" s="26"/>
@@ -4356,16 +4388,16 @@
       <c r="BR31" s="31"/>
     </row>
     <row r="32" spans="2:70" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="59"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="117"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="83"/>
-      <c r="G32" s="97"/>
-      <c r="H32" s="85"/>
-      <c r="I32" s="87"/>
-      <c r="J32" s="70"/>
-      <c r="K32" s="64"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="114"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="96"/>
+      <c r="H32" s="84"/>
+      <c r="I32" s="86"/>
+      <c r="J32" s="69"/>
+      <c r="K32" s="63"/>
       <c r="L32" s="34"/>
       <c r="M32" s="34"/>
       <c r="N32" s="34"/>
@@ -4449,20 +4481,6 @@
     <mergeCell ref="BD6:BH6"/>
     <mergeCell ref="BI6:BM6"/>
   </mergeCells>
-  <conditionalFormatting sqref="J11:J32 J8">
-    <cfRule type="dataBar" priority="6">
-      <dataBar>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="100"/>
-        <color theme="3" tint="0.59999389629810485"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{FE5B685F-D93A-1B44-AB73-D05D527007CF}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="J10">
     <cfRule type="dataBar" priority="4">
       <dataBar>
@@ -4491,26 +4509,25 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J11:J19 J8 J21:J32">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="100"/>
+        <color theme="3" tint="0.59999389629810485"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{FE5B685F-D93A-1B44-AB73-D05D527007CF}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FE5B685F-D93A-1B44-AB73-D05D527007CF}">
-            <x14:dataBar minLength="0" maxLength="100">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="percent">
-                <xm:f>100</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor theme="0"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>J11:J32 J8</xm:sqref>
-        </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A1D1EA57-9F10-4D4A-869C-EC4541125C39}">
             <x14:dataBar minLength="0" maxLength="100">
@@ -4541,6 +4558,21 @@
           </x14:cfRule>
           <xm:sqref>J9</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FE5B685F-D93A-1B44-AB73-D05D527007CF}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>100</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor theme="0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J11:J19 J8 J21:J32</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Uploading GDD Documentation V1.1
Signed-off-by: NorhanNassar <norhan.nassar96@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PP.xlsx
+++ b/SW deliveries log/PP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27636" yWindow="0" windowWidth="21504" windowHeight="9780" tabRatio="500"/>
+    <workbookView xWindow="29904" yWindow="0" windowWidth="21504" windowHeight="9780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Gantt Chart - BLANK" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="107">
   <si>
     <t>DURATION</t>
   </si>
@@ -312,28 +312,34 @@
     <t>Qandeel</t>
   </si>
   <si>
-    <t>28/2/2021</t>
-  </si>
-  <si>
-    <t>28/2/2022</t>
-  </si>
-  <si>
-    <t>28/2/2023</t>
-  </si>
-  <si>
-    <t>28/2/2024</t>
-  </si>
-  <si>
-    <t>29/2/2021</t>
-  </si>
-  <si>
-    <t>29/2/2022</t>
-  </si>
-  <si>
-    <t>29/2/2023</t>
-  </si>
-  <si>
-    <t>29/2/2024</t>
+    <t>19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRR Documetation </t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Updating Its Software Context Diagram</t>
+  </si>
+  <si>
+    <t>Updating whole documentation according to its Rewiew</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
   </si>
 </sst>
 </file>
@@ -567,7 +573,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="62">
+  <borders count="66">
     <border>
       <left/>
       <right/>
@@ -1172,21 +1178,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </left>
-      <right style="hair">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -1226,17 +1217,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="medium">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color theme="0" tint="-0.249977111117893"/>
       </right>
@@ -1363,6 +1343,90 @@
       <top/>
       <bottom style="thin">
         <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="hair">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="medium">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1372,7 +1436,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1476,34 +1540,13 @@
     <xf numFmtId="49" fontId="5" fillId="9" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="9" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1545,9 +1588,6 @@
     <xf numFmtId="14" fontId="5" fillId="8" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="5" fillId="8" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1557,19 +1597,10 @@
     <xf numFmtId="164" fontId="5" fillId="8" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="9" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1584,28 +1615,25 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="8" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="8" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="19" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="19" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="19" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1631,64 +1659,55 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="9" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="9" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="9" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1709,9 +1728,10 @@
     <xf numFmtId="0" fontId="5" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1784,7 +1804,30 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="8" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="8" borderId="65" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2012,9 +2055,9 @@
   </sheetPr>
   <dimension ref="B1:BR39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH26" sqref="AH26"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2054,22 +2097,22 @@
       <c r="U1" s="47"/>
     </row>
     <row r="2" spans="2:70" s="1" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="109"/>
+      <c r="D2" s="97"/>
     </row>
     <row r="3" spans="2:70" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="110"/>
+      <c r="D3" s="98"/>
     </row>
     <row r="4" spans="2:70" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
@@ -2084,74 +2127,74 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="141" t="s">
+      <c r="K5" s="127" t="s">
         <v>1</v>
       </c>
-      <c r="L5" s="142"/>
-      <c r="M5" s="142"/>
-      <c r="N5" s="142"/>
-      <c r="O5" s="142"/>
-      <c r="P5" s="142"/>
-      <c r="Q5" s="142"/>
-      <c r="R5" s="142"/>
-      <c r="S5" s="142"/>
-      <c r="T5" s="142"/>
-      <c r="U5" s="142"/>
-      <c r="V5" s="142"/>
-      <c r="W5" s="142"/>
-      <c r="X5" s="142"/>
-      <c r="Y5" s="143"/>
-      <c r="Z5" s="144" t="s">
+      <c r="L5" s="128"/>
+      <c r="M5" s="128"/>
+      <c r="N5" s="128"/>
+      <c r="O5" s="128"/>
+      <c r="P5" s="128"/>
+      <c r="Q5" s="128"/>
+      <c r="R5" s="128"/>
+      <c r="S5" s="128"/>
+      <c r="T5" s="128"/>
+      <c r="U5" s="128"/>
+      <c r="V5" s="128"/>
+      <c r="W5" s="128"/>
+      <c r="X5" s="128"/>
+      <c r="Y5" s="129"/>
+      <c r="Z5" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="AA5" s="145"/>
-      <c r="AB5" s="145"/>
-      <c r="AC5" s="145"/>
-      <c r="AD5" s="145"/>
-      <c r="AE5" s="145"/>
-      <c r="AF5" s="145"/>
-      <c r="AG5" s="145"/>
-      <c r="AH5" s="145"/>
-      <c r="AI5" s="145"/>
-      <c r="AJ5" s="145"/>
-      <c r="AK5" s="145"/>
-      <c r="AL5" s="145"/>
-      <c r="AM5" s="145"/>
-      <c r="AN5" s="146"/>
-      <c r="AO5" s="147" t="s">
+      <c r="AA5" s="131"/>
+      <c r="AB5" s="131"/>
+      <c r="AC5" s="131"/>
+      <c r="AD5" s="131"/>
+      <c r="AE5" s="131"/>
+      <c r="AF5" s="131"/>
+      <c r="AG5" s="131"/>
+      <c r="AH5" s="131"/>
+      <c r="AI5" s="131"/>
+      <c r="AJ5" s="131"/>
+      <c r="AK5" s="131"/>
+      <c r="AL5" s="131"/>
+      <c r="AM5" s="131"/>
+      <c r="AN5" s="132"/>
+      <c r="AO5" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="AP5" s="148"/>
-      <c r="AQ5" s="148"/>
-      <c r="AR5" s="148"/>
-      <c r="AS5" s="148"/>
-      <c r="AT5" s="148"/>
-      <c r="AU5" s="148"/>
-      <c r="AV5" s="148"/>
-      <c r="AW5" s="148"/>
-      <c r="AX5" s="148"/>
-      <c r="AY5" s="148"/>
-      <c r="AZ5" s="148"/>
-      <c r="BA5" s="148"/>
-      <c r="BB5" s="148"/>
-      <c r="BC5" s="149"/>
-      <c r="BD5" s="150" t="s">
+      <c r="AP5" s="134"/>
+      <c r="AQ5" s="134"/>
+      <c r="AR5" s="134"/>
+      <c r="AS5" s="134"/>
+      <c r="AT5" s="134"/>
+      <c r="AU5" s="134"/>
+      <c r="AV5" s="134"/>
+      <c r="AW5" s="134"/>
+      <c r="AX5" s="134"/>
+      <c r="AY5" s="134"/>
+      <c r="AZ5" s="134"/>
+      <c r="BA5" s="134"/>
+      <c r="BB5" s="134"/>
+      <c r="BC5" s="135"/>
+      <c r="BD5" s="136" t="s">
         <v>4</v>
       </c>
-      <c r="BE5" s="151"/>
-      <c r="BF5" s="151"/>
-      <c r="BG5" s="151"/>
-      <c r="BH5" s="151"/>
-      <c r="BI5" s="151"/>
-      <c r="BJ5" s="151"/>
-      <c r="BK5" s="151"/>
-      <c r="BL5" s="151"/>
-      <c r="BM5" s="151"/>
-      <c r="BN5" s="151"/>
-      <c r="BO5" s="151"/>
-      <c r="BP5" s="151"/>
-      <c r="BQ5" s="151"/>
-      <c r="BR5" s="152"/>
+      <c r="BE5" s="137"/>
+      <c r="BF5" s="137"/>
+      <c r="BG5" s="137"/>
+      <c r="BH5" s="137"/>
+      <c r="BI5" s="137"/>
+      <c r="BJ5" s="137"/>
+      <c r="BK5" s="137"/>
+      <c r="BL5" s="137"/>
+      <c r="BM5" s="137"/>
+      <c r="BN5" s="137"/>
+      <c r="BO5" s="137"/>
+      <c r="BP5" s="137"/>
+      <c r="BQ5" s="137"/>
+      <c r="BR5" s="138"/>
     </row>
     <row r="6" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
@@ -2166,105 +2209,105 @@
       <c r="E6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="87" t="s">
+      <c r="F6" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="91" t="s">
+      <c r="G6" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="88" t="s">
+      <c r="H6" s="77" t="s">
         <v>29</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="64" t="s">
+      <c r="J6" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="153" t="s">
+      <c r="K6" s="139" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="154"/>
-      <c r="M6" s="154"/>
-      <c r="N6" s="154"/>
-      <c r="O6" s="154"/>
-      <c r="P6" s="154" t="s">
+      <c r="L6" s="140"/>
+      <c r="M6" s="140"/>
+      <c r="N6" s="140"/>
+      <c r="O6" s="140"/>
+      <c r="P6" s="140" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="154"/>
-      <c r="R6" s="154"/>
-      <c r="S6" s="154"/>
-      <c r="T6" s="154"/>
-      <c r="U6" s="154" t="s">
+      <c r="Q6" s="140"/>
+      <c r="R6" s="140"/>
+      <c r="S6" s="140"/>
+      <c r="T6" s="140"/>
+      <c r="U6" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="V6" s="154"/>
-      <c r="W6" s="154"/>
-      <c r="X6" s="154"/>
-      <c r="Y6" s="155"/>
-      <c r="Z6" s="156" t="s">
+      <c r="V6" s="140"/>
+      <c r="W6" s="140"/>
+      <c r="X6" s="140"/>
+      <c r="Y6" s="141"/>
+      <c r="Z6" s="142" t="s">
         <v>8</v>
       </c>
-      <c r="AA6" s="157"/>
-      <c r="AB6" s="157"/>
-      <c r="AC6" s="157"/>
-      <c r="AD6" s="157"/>
-      <c r="AE6" s="157" t="s">
+      <c r="AA6" s="143"/>
+      <c r="AB6" s="143"/>
+      <c r="AC6" s="143"/>
+      <c r="AD6" s="143"/>
+      <c r="AE6" s="143" t="s">
         <v>9</v>
       </c>
-      <c r="AF6" s="157"/>
-      <c r="AG6" s="157"/>
-      <c r="AH6" s="157"/>
-      <c r="AI6" s="157"/>
-      <c r="AJ6" s="157" t="s">
+      <c r="AF6" s="143"/>
+      <c r="AG6" s="143"/>
+      <c r="AH6" s="143"/>
+      <c r="AI6" s="143"/>
+      <c r="AJ6" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="AK6" s="157"/>
-      <c r="AL6" s="157"/>
-      <c r="AM6" s="157"/>
-      <c r="AN6" s="158"/>
-      <c r="AO6" s="159" t="s">
+      <c r="AK6" s="143"/>
+      <c r="AL6" s="143"/>
+      <c r="AM6" s="143"/>
+      <c r="AN6" s="144"/>
+      <c r="AO6" s="145" t="s">
         <v>11</v>
       </c>
-      <c r="AP6" s="160"/>
-      <c r="AQ6" s="160"/>
-      <c r="AR6" s="160"/>
-      <c r="AS6" s="160"/>
-      <c r="AT6" s="160" t="s">
+      <c r="AP6" s="146"/>
+      <c r="AQ6" s="146"/>
+      <c r="AR6" s="146"/>
+      <c r="AS6" s="146"/>
+      <c r="AT6" s="146" t="s">
         <v>12</v>
       </c>
-      <c r="AU6" s="160"/>
-      <c r="AV6" s="160"/>
-      <c r="AW6" s="160"/>
-      <c r="AX6" s="160"/>
-      <c r="AY6" s="160" t="s">
+      <c r="AU6" s="146"/>
+      <c r="AV6" s="146"/>
+      <c r="AW6" s="146"/>
+      <c r="AX6" s="146"/>
+      <c r="AY6" s="146" t="s">
         <v>13</v>
       </c>
-      <c r="AZ6" s="160"/>
-      <c r="BA6" s="160"/>
-      <c r="BB6" s="160"/>
-      <c r="BC6" s="161"/>
-      <c r="BD6" s="162" t="s">
+      <c r="AZ6" s="146"/>
+      <c r="BA6" s="146"/>
+      <c r="BB6" s="146"/>
+      <c r="BC6" s="147"/>
+      <c r="BD6" s="148" t="s">
         <v>14</v>
       </c>
-      <c r="BE6" s="139"/>
-      <c r="BF6" s="139"/>
-      <c r="BG6" s="139"/>
-      <c r="BH6" s="139"/>
-      <c r="BI6" s="139" t="s">
+      <c r="BE6" s="125"/>
+      <c r="BF6" s="125"/>
+      <c r="BG6" s="125"/>
+      <c r="BH6" s="125"/>
+      <c r="BI6" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="BJ6" s="139"/>
-      <c r="BK6" s="139"/>
-      <c r="BL6" s="139"/>
-      <c r="BM6" s="139"/>
-      <c r="BN6" s="139" t="s">
+      <c r="BJ6" s="125"/>
+      <c r="BK6" s="125"/>
+      <c r="BL6" s="125"/>
+      <c r="BM6" s="125"/>
+      <c r="BN6" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="BO6" s="139"/>
-      <c r="BP6" s="139"/>
-      <c r="BQ6" s="139"/>
-      <c r="BR6" s="140"/>
+      <c r="BO6" s="125"/>
+      <c r="BP6" s="125"/>
+      <c r="BQ6" s="125"/>
+      <c r="BR6" s="126"/>
     </row>
     <row r="7" spans="2:70" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="9" t="s">
@@ -2279,19 +2322,19 @@
       <c r="E7" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="89" t="s">
+      <c r="F7" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="92" t="s">
+      <c r="G7" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="90" t="s">
+      <c r="H7" s="79" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="65" t="s">
+      <c r="J7" s="58" t="s">
         <v>30</v>
       </c>
       <c r="K7" s="12" t="s">
@@ -2479,33 +2522,33 @@
       <c r="B8" s="48">
         <v>1</v>
       </c>
-      <c r="C8" s="134" t="s">
+      <c r="C8" s="119" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="133" t="s">
+      <c r="D8" s="118" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="121" t="s">
+      <c r="E8" s="106" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="79" t="s">
+      <c r="F8" s="71" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="93" t="s">
+      <c r="G8" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="77" t="s">
+      <c r="H8" s="70" t="s">
         <v>41</v>
       </c>
       <c r="I8" s="49">
         <v>1</v>
       </c>
-      <c r="J8" s="66">
+      <c r="J8" s="59">
         <v>1</v>
       </c>
-      <c r="K8" s="61"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="108"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="96"/>
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
       <c r="P8" s="22"/>
@@ -2568,34 +2611,34 @@
       <c r="B9" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="135" t="s">
+      <c r="C9" s="120" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="133" t="s">
+      <c r="D9" s="118" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="121" t="s">
+      <c r="E9" s="106" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="79" t="s">
+      <c r="F9" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="93" t="s">
+      <c r="G9" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="77" t="s">
+      <c r="H9" s="70" t="s">
         <v>45</v>
       </c>
       <c r="I9" s="49">
         <v>1</v>
       </c>
-      <c r="J9" s="66">
+      <c r="J9" s="59">
         <v>1</v>
       </c>
-      <c r="K9" s="61"/>
-      <c r="L9" s="108"/>
-      <c r="M9" s="74"/>
-      <c r="N9" s="108"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="96"/>
+      <c r="M9" s="67"/>
+      <c r="N9" s="96"/>
       <c r="O9" s="22"/>
       <c r="P9" s="22"/>
       <c r="Q9" s="22"/>
@@ -2657,34 +2700,34 @@
       <c r="B10" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="134" t="s">
+      <c r="C10" s="119" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="133" t="s">
+      <c r="D10" s="118" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="121" t="s">
+      <c r="E10" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="79" t="s">
+      <c r="F10" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="93" t="s">
+      <c r="G10" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="77" t="s">
+      <c r="H10" s="70" t="s">
         <v>45</v>
       </c>
       <c r="I10" s="49">
         <v>1</v>
       </c>
-      <c r="J10" s="66">
+      <c r="J10" s="59">
         <v>1</v>
       </c>
-      <c r="K10" s="61"/>
-      <c r="L10" s="108"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="108"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="96"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="96"/>
       <c r="O10" s="22"/>
       <c r="P10" s="22"/>
       <c r="Q10" s="22"/>
@@ -2746,37 +2789,37 @@
       <c r="B11" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="136" t="s">
+      <c r="C11" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="111" t="s">
+      <c r="D11" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="119" t="s">
+      <c r="E11" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="80">
+      <c r="F11" s="72">
         <v>43892</v>
       </c>
-      <c r="G11" s="94">
+      <c r="G11" s="83">
         <v>43923</v>
       </c>
-      <c r="H11" s="94">
+      <c r="H11" s="83">
         <v>43923</v>
       </c>
-      <c r="I11" s="85">
+      <c r="I11" s="75">
         <v>1</v>
       </c>
-      <c r="J11" s="67">
+      <c r="J11" s="60">
         <v>1</v>
       </c>
-      <c r="K11" s="62"/>
+      <c r="K11" s="55"/>
       <c r="L11" s="26"/>
       <c r="M11" s="26"/>
       <c r="N11" s="26"/>
       <c r="O11" s="26"/>
-      <c r="P11" s="106"/>
-      <c r="Q11" s="107"/>
+      <c r="P11" s="94"/>
+      <c r="Q11" s="95"/>
       <c r="R11" s="27"/>
       <c r="S11" s="27"/>
       <c r="T11" s="27"/>
@@ -2835,37 +2878,37 @@
       <c r="B12" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="136" t="s">
+      <c r="C12" s="121" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="111" t="s">
+      <c r="D12" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="119" t="s">
+      <c r="E12" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="80">
+      <c r="F12" s="72">
         <v>43892</v>
       </c>
-      <c r="G12" s="94">
+      <c r="G12" s="83">
         <v>43923</v>
       </c>
-      <c r="H12" s="94">
+      <c r="H12" s="83">
         <v>43923</v>
       </c>
-      <c r="I12" s="85">
+      <c r="I12" s="75">
         <v>1</v>
       </c>
-      <c r="J12" s="67">
+      <c r="J12" s="60">
         <v>1</v>
       </c>
-      <c r="K12" s="62"/>
+      <c r="K12" s="55"/>
       <c r="L12" s="26"/>
       <c r="M12" s="26"/>
       <c r="N12" s="26"/>
       <c r="O12" s="26"/>
-      <c r="P12" s="74"/>
-      <c r="Q12" s="102"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="90"/>
       <c r="R12" s="27"/>
       <c r="S12" s="27"/>
       <c r="T12" s="27"/>
@@ -2924,38 +2967,38 @@
       <c r="B13" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="136" t="s">
+      <c r="C13" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="115" t="s">
+      <c r="D13" s="100" t="s">
         <v>75</v>
       </c>
-      <c r="E13" s="119" t="s">
+      <c r="E13" s="104" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="80">
+      <c r="F13" s="72">
         <v>43923</v>
       </c>
-      <c r="G13" s="94">
+      <c r="G13" s="83">
         <v>43953</v>
       </c>
-      <c r="H13" s="94">
+      <c r="H13" s="83">
         <v>43953</v>
       </c>
-      <c r="I13" s="85">
+      <c r="I13" s="75">
         <v>1</v>
       </c>
-      <c r="J13" s="67">
+      <c r="J13" s="60">
         <v>1</v>
       </c>
-      <c r="K13" s="62"/>
+      <c r="K13" s="55"/>
       <c r="L13" s="26"/>
       <c r="M13" s="26"/>
       <c r="N13" s="26"/>
       <c r="O13" s="26"/>
       <c r="P13" s="27"/>
-      <c r="Q13" s="74"/>
-      <c r="R13" s="102"/>
+      <c r="Q13" s="67"/>
+      <c r="R13" s="90"/>
       <c r="S13" s="27"/>
       <c r="T13" s="27"/>
       <c r="U13" s="26"/>
@@ -3013,38 +3056,38 @@
       <c r="B14" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="136" t="s">
+      <c r="C14" s="121" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="115" t="s">
+      <c r="D14" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="119" t="s">
+      <c r="E14" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="80">
+      <c r="F14" s="72">
         <v>43923</v>
       </c>
-      <c r="G14" s="94">
+      <c r="G14" s="83">
         <v>43953</v>
       </c>
-      <c r="H14" s="94">
+      <c r="H14" s="83">
         <v>43953</v>
       </c>
-      <c r="I14" s="85">
+      <c r="I14" s="75">
         <v>1</v>
       </c>
-      <c r="J14" s="67">
+      <c r="J14" s="60">
         <v>1</v>
       </c>
-      <c r="K14" s="62"/>
+      <c r="K14" s="55"/>
       <c r="L14" s="26"/>
       <c r="M14" s="26"/>
       <c r="N14" s="26"/>
       <c r="O14" s="26"/>
       <c r="P14" s="27"/>
-      <c r="Q14" s="74"/>
-      <c r="R14" s="102"/>
+      <c r="Q14" s="67"/>
+      <c r="R14" s="90"/>
       <c r="S14" s="27"/>
       <c r="T14" s="27"/>
       <c r="U14" s="26"/>
@@ -3102,40 +3145,40 @@
       <c r="B15" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="136" t="s">
+      <c r="C15" s="121" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="111" t="s">
+      <c r="D15" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="119" t="s">
+      <c r="E15" s="104" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="80">
+      <c r="F15" s="72">
         <v>43953</v>
       </c>
-      <c r="G15" s="94">
+      <c r="G15" s="83">
         <v>44014</v>
       </c>
-      <c r="H15" s="94">
+      <c r="H15" s="83">
         <v>44014</v>
       </c>
-      <c r="I15" s="85">
+      <c r="I15" s="75">
         <v>2</v>
       </c>
-      <c r="J15" s="67">
+      <c r="J15" s="60">
         <v>1</v>
       </c>
-      <c r="K15" s="62"/>
+      <c r="K15" s="55"/>
       <c r="L15" s="26"/>
       <c r="M15" s="26"/>
       <c r="N15" s="26"/>
       <c r="O15" s="26"/>
       <c r="P15" s="27"/>
       <c r="Q15" s="27"/>
-      <c r="R15" s="74"/>
-      <c r="S15" s="74"/>
-      <c r="T15" s="102"/>
+      <c r="R15" s="67"/>
+      <c r="S15" s="67"/>
+      <c r="T15" s="90"/>
       <c r="U15" s="26"/>
       <c r="V15" s="26"/>
       <c r="W15" s="26"/>
@@ -3191,120 +3234,120 @@
       <c r="B16" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="137" t="s">
+      <c r="C16" s="122" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="115" t="s">
+      <c r="D16" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="120" t="s">
+      <c r="E16" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="97">
+      <c r="F16" s="85">
         <v>44014</v>
       </c>
-      <c r="G16" s="98">
+      <c r="G16" s="86">
         <v>44045</v>
       </c>
-      <c r="H16" s="98">
+      <c r="H16" s="86">
         <v>44045</v>
       </c>
-      <c r="I16" s="99">
+      <c r="I16" s="87">
         <v>1</v>
       </c>
-      <c r="J16" s="100">
+      <c r="J16" s="88">
         <v>1</v>
       </c>
-      <c r="K16" s="101"/>
-      <c r="L16" s="102"/>
-      <c r="M16" s="102"/>
-      <c r="N16" s="102"/>
-      <c r="O16" s="102"/>
-      <c r="P16" s="102"/>
-      <c r="Q16" s="102"/>
-      <c r="R16" s="102"/>
-      <c r="S16" s="102"/>
-      <c r="T16" s="74"/>
-      <c r="U16" s="74"/>
-      <c r="V16" s="102"/>
-      <c r="W16" s="102"/>
-      <c r="X16" s="102"/>
-      <c r="Y16" s="103"/>
-      <c r="Z16" s="104"/>
-      <c r="AA16" s="102"/>
-      <c r="AB16" s="102"/>
-      <c r="AC16" s="102"/>
-      <c r="AD16" s="102"/>
-      <c r="AE16" s="102"/>
-      <c r="AF16" s="102"/>
-      <c r="AG16" s="102"/>
-      <c r="AH16" s="102"/>
-      <c r="AI16" s="102"/>
-      <c r="AJ16" s="102"/>
-      <c r="AK16" s="102"/>
-      <c r="AL16" s="102"/>
-      <c r="AM16" s="102"/>
-      <c r="AN16" s="103"/>
-      <c r="AO16" s="104"/>
-      <c r="AP16" s="102"/>
-      <c r="AQ16" s="102"/>
-      <c r="AR16" s="102"/>
-      <c r="AS16" s="102"/>
-      <c r="AT16" s="102"/>
-      <c r="AU16" s="102"/>
-      <c r="AV16" s="102"/>
-      <c r="AW16" s="102"/>
-      <c r="AX16" s="102"/>
-      <c r="AY16" s="102"/>
-      <c r="AZ16" s="102"/>
-      <c r="BA16" s="102"/>
-      <c r="BB16" s="102"/>
-      <c r="BC16" s="103"/>
-      <c r="BD16" s="104"/>
-      <c r="BE16" s="102"/>
-      <c r="BF16" s="102"/>
-      <c r="BG16" s="102"/>
-      <c r="BH16" s="102"/>
-      <c r="BI16" s="102"/>
-      <c r="BJ16" s="102"/>
-      <c r="BK16" s="102"/>
-      <c r="BL16" s="102"/>
-      <c r="BM16" s="102"/>
-      <c r="BN16" s="102"/>
-      <c r="BO16" s="102"/>
-      <c r="BP16" s="102"/>
-      <c r="BQ16" s="102"/>
-      <c r="BR16" s="105"/>
+      <c r="K16" s="89"/>
+      <c r="L16" s="90"/>
+      <c r="M16" s="90"/>
+      <c r="N16" s="90"/>
+      <c r="O16" s="90"/>
+      <c r="P16" s="90"/>
+      <c r="Q16" s="90"/>
+      <c r="R16" s="90"/>
+      <c r="S16" s="90"/>
+      <c r="T16" s="67"/>
+      <c r="U16" s="67"/>
+      <c r="V16" s="90"/>
+      <c r="W16" s="90"/>
+      <c r="X16" s="90"/>
+      <c r="Y16" s="91"/>
+      <c r="Z16" s="92"/>
+      <c r="AA16" s="90"/>
+      <c r="AB16" s="90"/>
+      <c r="AC16" s="90"/>
+      <c r="AD16" s="90"/>
+      <c r="AE16" s="90"/>
+      <c r="AF16" s="90"/>
+      <c r="AG16" s="90"/>
+      <c r="AH16" s="90"/>
+      <c r="AI16" s="90"/>
+      <c r="AJ16" s="90"/>
+      <c r="AK16" s="90"/>
+      <c r="AL16" s="90"/>
+      <c r="AM16" s="90"/>
+      <c r="AN16" s="91"/>
+      <c r="AO16" s="92"/>
+      <c r="AP16" s="90"/>
+      <c r="AQ16" s="90"/>
+      <c r="AR16" s="90"/>
+      <c r="AS16" s="90"/>
+      <c r="AT16" s="90"/>
+      <c r="AU16" s="90"/>
+      <c r="AV16" s="90"/>
+      <c r="AW16" s="90"/>
+      <c r="AX16" s="90"/>
+      <c r="AY16" s="90"/>
+      <c r="AZ16" s="90"/>
+      <c r="BA16" s="90"/>
+      <c r="BB16" s="90"/>
+      <c r="BC16" s="91"/>
+      <c r="BD16" s="92"/>
+      <c r="BE16" s="90"/>
+      <c r="BF16" s="90"/>
+      <c r="BG16" s="90"/>
+      <c r="BH16" s="90"/>
+      <c r="BI16" s="90"/>
+      <c r="BJ16" s="90"/>
+      <c r="BK16" s="90"/>
+      <c r="BL16" s="90"/>
+      <c r="BM16" s="90"/>
+      <c r="BN16" s="90"/>
+      <c r="BO16" s="90"/>
+      <c r="BP16" s="90"/>
+      <c r="BQ16" s="90"/>
+      <c r="BR16" s="93"/>
     </row>
     <row r="17" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="136" t="s">
+      <c r="C17" s="121" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="111" t="s">
+      <c r="D17" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="119" t="s">
+      <c r="E17" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="97" t="s">
+      <c r="F17" s="85" t="s">
         <v>70</v>
       </c>
-      <c r="G17" s="98" t="s">
+      <c r="G17" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="98" t="s">
+      <c r="H17" s="86" t="s">
         <v>69</v>
       </c>
-      <c r="I17" s="85">
+      <c r="I17" s="75">
         <v>1</v>
       </c>
-      <c r="J17" s="67">
+      <c r="J17" s="60">
         <v>1</v>
       </c>
-      <c r="K17" s="62"/>
+      <c r="K17" s="55"/>
       <c r="L17" s="26"/>
       <c r="M17" s="26"/>
       <c r="N17" s="26"/>
@@ -3316,11 +3359,11 @@
       <c r="T17" s="27"/>
       <c r="U17" s="26"/>
       <c r="V17" s="26"/>
-      <c r="W17" s="74"/>
-      <c r="X17" s="74"/>
+      <c r="W17" s="67"/>
+      <c r="X17" s="67"/>
       <c r="Y17" s="28"/>
       <c r="Z17" s="25"/>
-      <c r="AA17" s="102"/>
+      <c r="AA17" s="90"/>
       <c r="AB17" s="26"/>
       <c r="AC17" s="26"/>
       <c r="AD17" s="26"/>
@@ -3369,31 +3412,31 @@
       <c r="B18" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="136" t="s">
+      <c r="C18" s="121" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="116" t="s">
+      <c r="D18" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="E18" s="119" t="s">
+      <c r="E18" s="104" t="s">
         <v>59</v>
       </c>
-      <c r="F18" s="97" t="s">
+      <c r="F18" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="G18" s="97" t="s">
+      <c r="G18" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="83" t="s">
+      <c r="H18" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="I18" s="85">
+      <c r="I18" s="75">
         <v>1</v>
       </c>
-      <c r="J18" s="67">
+      <c r="J18" s="60">
         <v>1</v>
       </c>
-      <c r="K18" s="62"/>
+      <c r="K18" s="55"/>
       <c r="L18" s="26"/>
       <c r="M18" s="26"/>
       <c r="N18" s="26"/>
@@ -3406,8 +3449,8 @@
       <c r="U18" s="26"/>
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
-      <c r="X18" s="74"/>
-      <c r="Y18" s="74"/>
+      <c r="X18" s="67"/>
+      <c r="Y18" s="67"/>
       <c r="Z18" s="25"/>
       <c r="AA18" s="26"/>
       <c r="AB18" s="26"/>
@@ -3455,34 +3498,34 @@
       <c r="BR18" s="31"/>
     </row>
     <row r="19" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="129" t="s">
+      <c r="B19" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="138" t="s">
+      <c r="C19" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="117" t="s">
+      <c r="D19" s="102" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="116" t="s">
+      <c r="E19" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="122" t="s">
+      <c r="F19" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="123" t="s">
+      <c r="G19" s="108" t="s">
         <v>81</v>
       </c>
-      <c r="H19" s="83" t="s">
+      <c r="H19" s="74" t="s">
         <v>69</v>
       </c>
-      <c r="I19" s="124">
+      <c r="I19" s="109">
         <v>1</v>
       </c>
-      <c r="J19" s="125">
+      <c r="J19" s="110">
         <v>1</v>
       </c>
-      <c r="K19" s="62"/>
+      <c r="K19" s="55"/>
       <c r="L19" s="26"/>
       <c r="M19" s="26"/>
       <c r="N19" s="26"/>
@@ -3545,11 +3588,11 @@
     </row>
     <row r="20" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="48"/>
-      <c r="C20" s="130"/>
-      <c r="D20" s="118" t="s">
+      <c r="C20" s="115"/>
+      <c r="D20" s="103" t="s">
         <v>79</v>
       </c>
-      <c r="K20" s="62"/>
+      <c r="K20" s="55"/>
       <c r="L20" s="26"/>
       <c r="M20" s="26"/>
       <c r="N20" s="26"/>
@@ -3614,31 +3657,31 @@
       <c r="B21" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="132" t="s">
+      <c r="C21" s="117" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="133" t="s">
+      <c r="D21" s="118" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="131" t="s">
+      <c r="E21" s="116" t="s">
         <v>82</v>
       </c>
-      <c r="F21" s="126" t="s">
+      <c r="F21" s="111" t="s">
         <v>83</v>
       </c>
-      <c r="G21" s="126" t="s">
+      <c r="G21" s="111" t="s">
         <v>84</v>
       </c>
-      <c r="H21" s="126" t="s">
+      <c r="H21" s="111" t="s">
         <v>84</v>
       </c>
-      <c r="I21" s="127">
+      <c r="I21" s="112">
         <v>1</v>
       </c>
-      <c r="J21" s="128">
+      <c r="J21" s="113">
         <v>1</v>
       </c>
-      <c r="K21" s="61"/>
+      <c r="K21" s="54"/>
       <c r="L21" s="22"/>
       <c r="M21" s="22"/>
       <c r="N21" s="22"/>
@@ -3660,7 +3703,7 @@
       <c r="AD21" s="22"/>
       <c r="AE21" s="22"/>
       <c r="AF21" s="22"/>
-      <c r="AG21" s="163"/>
+      <c r="AG21" s="124"/>
       <c r="AH21" s="22"/>
       <c r="AI21" s="22"/>
       <c r="AJ21" s="22"/>
@@ -3703,29 +3746,31 @@
       <c r="B22" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="136" t="s">
+      <c r="C22" s="121" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="115" t="s">
+      <c r="D22" s="100" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="116" t="s">
+      <c r="E22" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="81" t="s">
+      <c r="F22" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="G22" s="95" t="s">
+      <c r="G22" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="H22" s="83"/>
-      <c r="I22" s="57">
+      <c r="H22" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="I22" s="52">
         <v>1</v>
       </c>
-      <c r="J22" s="68">
-        <v>0.5</v>
-      </c>
-      <c r="K22" s="62"/>
+      <c r="J22" s="61">
+        <v>1</v>
+      </c>
+      <c r="K22" s="55"/>
       <c r="L22" s="26"/>
       <c r="M22" s="26"/>
       <c r="N22" s="26"/>
@@ -3748,7 +3793,7 @@
       <c r="AE22" s="29"/>
       <c r="AF22" s="29"/>
       <c r="AG22" s="29"/>
-      <c r="AH22" s="163"/>
+      <c r="AH22" s="124"/>
       <c r="AI22" s="29"/>
       <c r="AJ22" s="26"/>
       <c r="AK22" s="26"/>
@@ -3756,7 +3801,7 @@
       <c r="AM22" s="26"/>
       <c r="AN22" s="28"/>
       <c r="AO22" s="25"/>
-      <c r="AP22" s="75"/>
+      <c r="AP22" s="68"/>
       <c r="AQ22" s="26"/>
       <c r="AR22" s="26"/>
       <c r="AS22" s="26"/>
@@ -3790,29 +3835,31 @@
       <c r="B23" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="136" t="s">
+      <c r="C23" s="121" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="115" t="s">
+      <c r="D23" s="100" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="119" t="s">
+      <c r="E23" s="104" t="s">
         <v>59</v>
       </c>
-      <c r="F23" s="81" t="s">
-        <v>97</v>
-      </c>
-      <c r="G23" s="95" t="s">
-        <v>101</v>
-      </c>
-      <c r="H23" s="83"/>
-      <c r="I23" s="57">
+      <c r="F23" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="H23" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="I23" s="52">
         <v>1</v>
       </c>
-      <c r="J23" s="67">
-        <v>0</v>
-      </c>
-      <c r="K23" s="62"/>
+      <c r="J23" s="60">
+        <v>1</v>
+      </c>
+      <c r="K23" s="55"/>
       <c r="L23" s="26"/>
       <c r="M23" s="26"/>
       <c r="N23" s="26"/>
@@ -3835,7 +3882,7 @@
       <c r="AE23" s="29"/>
       <c r="AF23" s="29"/>
       <c r="AG23" s="29"/>
-      <c r="AH23" s="163"/>
+      <c r="AH23" s="124"/>
       <c r="AI23" s="29"/>
       <c r="AJ23" s="26"/>
       <c r="AK23" s="26"/>
@@ -3877,29 +3924,31 @@
       <c r="B24" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="136" t="s">
+      <c r="C24" s="121" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="115" t="s">
+      <c r="D24" s="100" t="s">
         <v>89</v>
       </c>
-      <c r="E24" s="119" t="s">
+      <c r="E24" s="104" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="81" t="s">
-        <v>98</v>
-      </c>
-      <c r="G24" s="95" t="s">
-        <v>102</v>
-      </c>
-      <c r="H24" s="83"/>
-      <c r="I24" s="57">
+      <c r="F24" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="I24" s="52">
         <v>1</v>
       </c>
-      <c r="J24" s="67">
-        <v>0</v>
-      </c>
-      <c r="K24" s="62"/>
+      <c r="J24" s="60">
+        <v>1</v>
+      </c>
+      <c r="K24" s="55"/>
       <c r="L24" s="26"/>
       <c r="M24" s="26"/>
       <c r="N24" s="26"/>
@@ -3922,7 +3971,7 @@
       <c r="AE24" s="29"/>
       <c r="AF24" s="29"/>
       <c r="AG24" s="29"/>
-      <c r="AH24" s="163"/>
+      <c r="AH24" s="124"/>
       <c r="AI24" s="29"/>
       <c r="AJ24" s="26"/>
       <c r="AK24" s="26"/>
@@ -3964,29 +4013,31 @@
       <c r="B25" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="136" t="s">
+      <c r="C25" s="121" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="115" t="s">
+      <c r="D25" s="100" t="s">
         <v>89</v>
       </c>
-      <c r="E25" s="119" t="s">
+      <c r="E25" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="81" t="s">
-        <v>99</v>
-      </c>
-      <c r="G25" s="95" t="s">
-        <v>103</v>
-      </c>
-      <c r="H25" s="83"/>
-      <c r="I25" s="57">
+      <c r="F25" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="G25" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="H25" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="I25" s="52">
         <v>1</v>
       </c>
-      <c r="J25" s="67">
-        <v>0</v>
-      </c>
-      <c r="K25" s="62"/>
+      <c r="J25" s="60">
+        <v>1</v>
+      </c>
+      <c r="K25" s="55"/>
       <c r="L25" s="26"/>
       <c r="M25" s="26"/>
       <c r="N25" s="26"/>
@@ -4011,7 +4062,7 @@
       <c r="AE25" s="29"/>
       <c r="AF25" s="29"/>
       <c r="AG25" s="29"/>
-      <c r="AH25" s="163"/>
+      <c r="AH25" s="124"/>
       <c r="AI25" s="29"/>
       <c r="AJ25" s="26"/>
       <c r="AK25" s="26"/>
@@ -4053,29 +4104,31 @@
       <c r="B26" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="136" t="s">
+      <c r="C26" s="121" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="115" t="s">
+      <c r="D26" s="100" t="s">
         <v>89</v>
       </c>
-      <c r="E26" s="119" t="s">
+      <c r="E26" s="104" t="s">
         <v>96</v>
       </c>
-      <c r="F26" s="81" t="s">
-        <v>100</v>
-      </c>
-      <c r="G26" s="95" t="s">
-        <v>104</v>
-      </c>
-      <c r="H26" s="83"/>
-      <c r="I26" s="57">
+      <c r="F26" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="I26" s="52">
         <v>1</v>
       </c>
-      <c r="J26" s="67">
-        <v>0</v>
-      </c>
-      <c r="K26" s="62"/>
+      <c r="J26" s="60">
+        <v>1</v>
+      </c>
+      <c r="K26" s="55"/>
       <c r="L26" s="26"/>
       <c r="M26" s="26"/>
       <c r="N26" s="26"/>
@@ -4098,7 +4151,7 @@
       <c r="AE26" s="29"/>
       <c r="AF26" s="29"/>
       <c r="AG26" s="29"/>
-      <c r="AH26" s="163"/>
+      <c r="AH26" s="124"/>
       <c r="AI26" s="29"/>
       <c r="AJ26" s="26"/>
       <c r="AK26" s="26"/>
@@ -4137,16 +4190,34 @@
       <c r="BR26" s="31"/>
     </row>
     <row r="27" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="50"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="113"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="80"/>
-      <c r="G27" s="94"/>
-      <c r="H27" s="83"/>
-      <c r="I27" s="85"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="62"/>
+      <c r="B27" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="121" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="100" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="I27" s="75">
+        <v>1</v>
+      </c>
+      <c r="J27" s="60">
+        <v>1</v>
+      </c>
+      <c r="K27" s="55"/>
       <c r="L27" s="26"/>
       <c r="M27" s="26"/>
       <c r="N27" s="26"/>
@@ -4208,16 +4279,34 @@
       <c r="BR27" s="31"/>
     </row>
     <row r="28" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="50"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="112"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="81"/>
-      <c r="G28" s="95"/>
-      <c r="H28" s="78"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="61"/>
+      <c r="B28" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="156" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="149" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="150" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" s="151">
+        <v>43833</v>
+      </c>
+      <c r="G28" s="152">
+        <v>43864</v>
+      </c>
+      <c r="H28" s="153">
+        <v>43864</v>
+      </c>
+      <c r="I28" s="154">
+        <v>1</v>
+      </c>
+      <c r="J28" s="155">
+        <v>1</v>
+      </c>
+      <c r="K28" s="54"/>
       <c r="L28" s="22"/>
       <c r="M28" s="22"/>
       <c r="N28" s="22"/>
@@ -4279,16 +4368,34 @@
       <c r="BR28" s="24"/>
     </row>
     <row r="29" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="50"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="111"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="80"/>
-      <c r="G29" s="94"/>
-      <c r="H29" s="83"/>
-      <c r="I29" s="85"/>
-      <c r="J29" s="67"/>
-      <c r="K29" s="62"/>
+      <c r="B29" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="121" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="100" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="101" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="151">
+        <v>43864</v>
+      </c>
+      <c r="G29" s="152">
+        <v>43864</v>
+      </c>
+      <c r="H29" s="153">
+        <v>43864</v>
+      </c>
+      <c r="I29" s="154">
+        <v>1</v>
+      </c>
+      <c r="J29" s="113">
+        <v>0</v>
+      </c>
+      <c r="K29" s="55"/>
       <c r="L29" s="26"/>
       <c r="M29" s="26"/>
       <c r="N29" s="26"/>
@@ -4334,7 +4441,7 @@
       <c r="BB29" s="26"/>
       <c r="BC29" s="28"/>
       <c r="BD29" s="25"/>
-      <c r="BE29" s="76"/>
+      <c r="BE29" s="69"/>
       <c r="BF29" s="26"/>
       <c r="BG29" s="26"/>
       <c r="BH29" s="26"/>
@@ -4350,16 +4457,34 @@
       <c r="BR29" s="31"/>
     </row>
     <row r="30" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="50"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="111"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="80"/>
-      <c r="G30" s="94"/>
-      <c r="H30" s="83"/>
-      <c r="I30" s="85"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="62"/>
+      <c r="B30" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="121" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="100" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="104" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" s="151">
+        <v>43864</v>
+      </c>
+      <c r="G30" s="152">
+        <v>43864</v>
+      </c>
+      <c r="H30" s="153">
+        <v>43864</v>
+      </c>
+      <c r="I30" s="154">
+        <v>1</v>
+      </c>
+      <c r="J30" s="60">
+        <v>0</v>
+      </c>
+      <c r="K30" s="55"/>
       <c r="L30" s="26"/>
       <c r="M30" s="26"/>
       <c r="N30" s="26"/>
@@ -4421,16 +4546,34 @@
       <c r="BR30" s="31"/>
     </row>
     <row r="31" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="50"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="111"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="80"/>
-      <c r="G31" s="94"/>
-      <c r="H31" s="83"/>
-      <c r="I31" s="85"/>
-      <c r="J31" s="67"/>
-      <c r="K31" s="62"/>
+      <c r="B31" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="121" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="100" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" s="104" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" s="151">
+        <v>43864</v>
+      </c>
+      <c r="G31" s="152">
+        <v>43864</v>
+      </c>
+      <c r="H31" s="153">
+        <v>43864</v>
+      </c>
+      <c r="I31" s="154">
+        <v>1</v>
+      </c>
+      <c r="J31" s="60">
+        <v>0</v>
+      </c>
+      <c r="K31" s="55"/>
       <c r="L31" s="26"/>
       <c r="M31" s="26"/>
       <c r="N31" s="26"/>
@@ -4492,16 +4635,34 @@
       <c r="BR31" s="31"/>
     </row>
     <row r="32" spans="2:70" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="58"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="114"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="82"/>
-      <c r="G32" s="96"/>
-      <c r="H32" s="84"/>
-      <c r="I32" s="86"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="63"/>
+      <c r="B32" s="53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="121" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="100" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" s="104" t="s">
+        <v>40</v>
+      </c>
+      <c r="F32" s="151">
+        <v>43864</v>
+      </c>
+      <c r="G32" s="152">
+        <v>43864</v>
+      </c>
+      <c r="H32" s="153">
+        <v>43864</v>
+      </c>
+      <c r="I32" s="154">
+        <v>1</v>
+      </c>
+      <c r="J32" s="62">
+        <v>0</v>
+      </c>
+      <c r="K32" s="56"/>
       <c r="L32" s="34"/>
       <c r="M32" s="34"/>
       <c r="N32" s="34"/>
@@ -4562,7 +4723,36 @@
       <c r="BQ32" s="34"/>
       <c r="BR32" s="39"/>
     </row>
-    <row r="39" spans="3:4" ht="19.2" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="121" t="s">
+        <v>90</v>
+      </c>
+      <c r="D33" s="100" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="104" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="151">
+        <v>43864</v>
+      </c>
+      <c r="G33" s="152">
+        <v>43864</v>
+      </c>
+      <c r="H33" s="153">
+        <v>43864</v>
+      </c>
+      <c r="I33" s="154">
+        <v>1</v>
+      </c>
+      <c r="J33" s="62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" ht="19.2" x14ac:dyDescent="0.35">
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
@@ -4586,7 +4776,7 @@
     <mergeCell ref="BI6:BM6"/>
   </mergeCells>
   <conditionalFormatting sqref="J10">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -4600,7 +4790,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -4614,7 +4804,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:J19 J8 J21:J32">
-    <cfRule type="dataBar" priority="7">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="100"/>
@@ -4623,6 +4813,20 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{FE5B685F-D93A-1B44-AB73-D05D527007CF}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J33">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="100"/>
+        <color theme="3" tint="0.59999389629810485"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7EA5A9D1-6D48-4832-957C-36A6C3ACDA52}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -4677,6 +4881,21 @@
           </x14:cfRule>
           <xm:sqref>J11:J19 J8 J21:J32</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7EA5A9D1-6D48-4832-957C-36A6C3ACDA52}">
+            <x14:dataBar minLength="0" maxLength="100">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>100</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor theme="0"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J33</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
updating GDD Document and PP
Signed-off-by: NorhanNassar <norhan.nassar96@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PP.xlsx
+++ b/SW deliveries log/PP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="36708" yWindow="0" windowWidth="21504" windowHeight="9780" tabRatio="500"/>
+    <workbookView xWindow="38976" yWindow="0" windowWidth="21504" windowHeight="9780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Gantt Chart - BLANK" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="132">
   <si>
     <t>DURATION</t>
   </si>
@@ -397,6 +397,24 @@
   </si>
   <si>
     <t xml:space="preserve">Updating RTM according to new requirements </t>
+  </si>
+  <si>
+    <t>14/3/2020</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>Technical Cross Review</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>Cross Review</t>
   </si>
 </sst>
 </file>
@@ -1900,78 +1918,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1985,6 +1931,78 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2212,11 +2230,11 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:BR45"/>
+  <dimension ref="B1:BR48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
+      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2286,74 +2304,74 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="143" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="144"/>
-      <c r="M5" s="144"/>
-      <c r="N5" s="144"/>
-      <c r="O5" s="144"/>
-      <c r="P5" s="144"/>
-      <c r="Q5" s="144"/>
-      <c r="R5" s="144"/>
-      <c r="S5" s="144"/>
-      <c r="T5" s="144"/>
-      <c r="U5" s="144"/>
-      <c r="V5" s="144"/>
-      <c r="W5" s="144"/>
-      <c r="X5" s="144"/>
-      <c r="Y5" s="145"/>
-      <c r="Z5" s="146" t="s">
+      <c r="K5" s="148" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="149"/>
+      <c r="M5" s="149"/>
+      <c r="N5" s="149"/>
+      <c r="O5" s="149"/>
+      <c r="P5" s="149"/>
+      <c r="Q5" s="149"/>
+      <c r="R5" s="149"/>
+      <c r="S5" s="149"/>
+      <c r="T5" s="149"/>
+      <c r="U5" s="149"/>
+      <c r="V5" s="149"/>
+      <c r="W5" s="149"/>
+      <c r="X5" s="149"/>
+      <c r="Y5" s="150"/>
+      <c r="Z5" s="151" t="s">
         <v>2</v>
       </c>
-      <c r="AA5" s="147"/>
-      <c r="AB5" s="147"/>
-      <c r="AC5" s="147"/>
-      <c r="AD5" s="147"/>
-      <c r="AE5" s="147"/>
-      <c r="AF5" s="147"/>
-      <c r="AG5" s="147"/>
-      <c r="AH5" s="147"/>
-      <c r="AI5" s="147"/>
-      <c r="AJ5" s="147"/>
-      <c r="AK5" s="147"/>
-      <c r="AL5" s="147"/>
-      <c r="AM5" s="147"/>
-      <c r="AN5" s="148"/>
-      <c r="AO5" s="149" t="s">
+      <c r="AA5" s="152"/>
+      <c r="AB5" s="152"/>
+      <c r="AC5" s="152"/>
+      <c r="AD5" s="152"/>
+      <c r="AE5" s="152"/>
+      <c r="AF5" s="152"/>
+      <c r="AG5" s="152"/>
+      <c r="AH5" s="152"/>
+      <c r="AI5" s="152"/>
+      <c r="AJ5" s="152"/>
+      <c r="AK5" s="152"/>
+      <c r="AL5" s="152"/>
+      <c r="AM5" s="152"/>
+      <c r="AN5" s="153"/>
+      <c r="AO5" s="154" t="s">
         <v>3</v>
       </c>
-      <c r="AP5" s="150"/>
-      <c r="AQ5" s="150"/>
-      <c r="AR5" s="150"/>
-      <c r="AS5" s="150"/>
-      <c r="AT5" s="150"/>
-      <c r="AU5" s="150"/>
-      <c r="AV5" s="150"/>
-      <c r="AW5" s="150"/>
-      <c r="AX5" s="150"/>
-      <c r="AY5" s="150"/>
-      <c r="AZ5" s="150"/>
-      <c r="BA5" s="150"/>
-      <c r="BB5" s="150"/>
-      <c r="BC5" s="151"/>
-      <c r="BD5" s="152" t="s">
+      <c r="AP5" s="155"/>
+      <c r="AQ5" s="155"/>
+      <c r="AR5" s="155"/>
+      <c r="AS5" s="155"/>
+      <c r="AT5" s="155"/>
+      <c r="AU5" s="155"/>
+      <c r="AV5" s="155"/>
+      <c r="AW5" s="155"/>
+      <c r="AX5" s="155"/>
+      <c r="AY5" s="155"/>
+      <c r="AZ5" s="155"/>
+      <c r="BA5" s="155"/>
+      <c r="BB5" s="155"/>
+      <c r="BC5" s="156"/>
+      <c r="BD5" s="157" t="s">
         <v>4</v>
       </c>
-      <c r="BE5" s="153"/>
-      <c r="BF5" s="153"/>
-      <c r="BG5" s="153"/>
-      <c r="BH5" s="153"/>
-      <c r="BI5" s="153"/>
-      <c r="BJ5" s="153"/>
-      <c r="BK5" s="153"/>
-      <c r="BL5" s="153"/>
-      <c r="BM5" s="153"/>
-      <c r="BN5" s="153"/>
-      <c r="BO5" s="153"/>
-      <c r="BP5" s="153"/>
-      <c r="BQ5" s="153"/>
-      <c r="BR5" s="154"/>
+      <c r="BE5" s="158"/>
+      <c r="BF5" s="158"/>
+      <c r="BG5" s="158"/>
+      <c r="BH5" s="158"/>
+      <c r="BI5" s="158"/>
+      <c r="BJ5" s="158"/>
+      <c r="BK5" s="158"/>
+      <c r="BL5" s="158"/>
+      <c r="BM5" s="158"/>
+      <c r="BN5" s="158"/>
+      <c r="BO5" s="158"/>
+      <c r="BP5" s="158"/>
+      <c r="BQ5" s="158"/>
+      <c r="BR5" s="159"/>
     </row>
     <row r="6" spans="2:70" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
@@ -2383,90 +2401,90 @@
       <c r="J6" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="K6" s="155" t="s">
+      <c r="K6" s="160" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="156"/>
-      <c r="M6" s="156"/>
-      <c r="N6" s="156"/>
-      <c r="O6" s="156"/>
-      <c r="P6" s="156" t="s">
+      <c r="L6" s="161"/>
+      <c r="M6" s="161"/>
+      <c r="N6" s="161"/>
+      <c r="O6" s="161"/>
+      <c r="P6" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="156"/>
-      <c r="R6" s="156"/>
-      <c r="S6" s="156"/>
-      <c r="T6" s="156"/>
-      <c r="U6" s="156" t="s">
+      <c r="Q6" s="161"/>
+      <c r="R6" s="161"/>
+      <c r="S6" s="161"/>
+      <c r="T6" s="161"/>
+      <c r="U6" s="161" t="s">
         <v>7</v>
       </c>
-      <c r="V6" s="156"/>
-      <c r="W6" s="156"/>
-      <c r="X6" s="156"/>
-      <c r="Y6" s="157"/>
-      <c r="Z6" s="158" t="s">
+      <c r="V6" s="161"/>
+      <c r="W6" s="161"/>
+      <c r="X6" s="161"/>
+      <c r="Y6" s="162"/>
+      <c r="Z6" s="163" t="s">
         <v>8</v>
       </c>
-      <c r="AA6" s="159"/>
-      <c r="AB6" s="159"/>
-      <c r="AC6" s="159"/>
-      <c r="AD6" s="159"/>
-      <c r="AE6" s="159" t="s">
+      <c r="AA6" s="164"/>
+      <c r="AB6" s="164"/>
+      <c r="AC6" s="164"/>
+      <c r="AD6" s="164"/>
+      <c r="AE6" s="164" t="s">
         <v>9</v>
       </c>
-      <c r="AF6" s="159"/>
-      <c r="AG6" s="159"/>
-      <c r="AH6" s="159"/>
-      <c r="AI6" s="159"/>
-      <c r="AJ6" s="159" t="s">
+      <c r="AF6" s="164"/>
+      <c r="AG6" s="164"/>
+      <c r="AH6" s="164"/>
+      <c r="AI6" s="164"/>
+      <c r="AJ6" s="164" t="s">
         <v>10</v>
       </c>
-      <c r="AK6" s="159"/>
-      <c r="AL6" s="159"/>
-      <c r="AM6" s="159"/>
-      <c r="AN6" s="160"/>
-      <c r="AO6" s="161" t="s">
+      <c r="AK6" s="164"/>
+      <c r="AL6" s="164"/>
+      <c r="AM6" s="164"/>
+      <c r="AN6" s="165"/>
+      <c r="AO6" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="AP6" s="162"/>
-      <c r="AQ6" s="162"/>
-      <c r="AR6" s="162"/>
-      <c r="AS6" s="162"/>
-      <c r="AT6" s="162" t="s">
+      <c r="AP6" s="167"/>
+      <c r="AQ6" s="167"/>
+      <c r="AR6" s="167"/>
+      <c r="AS6" s="167"/>
+      <c r="AT6" s="167" t="s">
         <v>12</v>
       </c>
-      <c r="AU6" s="162"/>
-      <c r="AV6" s="162"/>
-      <c r="AW6" s="162"/>
-      <c r="AX6" s="162"/>
-      <c r="AY6" s="162" t="s">
+      <c r="AU6" s="167"/>
+      <c r="AV6" s="167"/>
+      <c r="AW6" s="167"/>
+      <c r="AX6" s="167"/>
+      <c r="AY6" s="167" t="s">
         <v>13</v>
       </c>
-      <c r="AZ6" s="162"/>
-      <c r="BA6" s="162"/>
-      <c r="BB6" s="162"/>
-      <c r="BC6" s="163"/>
-      <c r="BD6" s="164" t="s">
+      <c r="AZ6" s="167"/>
+      <c r="BA6" s="167"/>
+      <c r="BB6" s="167"/>
+      <c r="BC6" s="168"/>
+      <c r="BD6" s="169" t="s">
         <v>14</v>
       </c>
-      <c r="BE6" s="141"/>
-      <c r="BF6" s="141"/>
-      <c r="BG6" s="141"/>
-      <c r="BH6" s="141"/>
-      <c r="BI6" s="141" t="s">
+      <c r="BE6" s="146"/>
+      <c r="BF6" s="146"/>
+      <c r="BG6" s="146"/>
+      <c r="BH6" s="146"/>
+      <c r="BI6" s="146" t="s">
         <v>15</v>
       </c>
-      <c r="BJ6" s="141"/>
-      <c r="BK6" s="141"/>
-      <c r="BL6" s="141"/>
-      <c r="BM6" s="141"/>
-      <c r="BN6" s="141" t="s">
+      <c r="BJ6" s="146"/>
+      <c r="BK6" s="146"/>
+      <c r="BL6" s="146"/>
+      <c r="BM6" s="146"/>
+      <c r="BN6" s="146" t="s">
         <v>16</v>
       </c>
-      <c r="BO6" s="141"/>
-      <c r="BP6" s="141"/>
-      <c r="BQ6" s="141"/>
-      <c r="BR6" s="142"/>
+      <c r="BO6" s="146"/>
+      <c r="BP6" s="146"/>
+      <c r="BQ6" s="146"/>
+      <c r="BR6" s="147"/>
     </row>
     <row r="7" spans="2:70" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="9" t="s">
@@ -4973,107 +4991,115 @@
       <c r="B36" s="132" t="s">
         <v>112</v>
       </c>
-      <c r="C36" s="165" t="s">
+      <c r="C36" s="141" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="165" t="s">
+      <c r="D36" s="141" t="s">
         <v>113</v>
       </c>
-      <c r="E36" s="166" t="s">
+      <c r="E36" s="142" t="s">
         <v>82</v>
       </c>
-      <c r="F36" s="167">
+      <c r="F36" s="143">
         <v>44077</v>
       </c>
-      <c r="G36" s="167">
+      <c r="G36" s="143">
         <v>44107</v>
       </c>
-      <c r="H36" s="167"/>
-      <c r="I36" s="168">
-        <v>1</v>
-      </c>
-      <c r="J36" s="169">
-        <v>0</v>
+      <c r="H36" s="143">
+        <v>44168</v>
+      </c>
+      <c r="I36" s="144">
+        <v>1</v>
+      </c>
+      <c r="J36" s="145">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B37" s="132" t="s">
         <v>114</v>
       </c>
-      <c r="C37" s="165" t="s">
+      <c r="C37" s="141" t="s">
         <v>115</v>
       </c>
-      <c r="D37" s="165" t="s">
+      <c r="D37" s="141" t="s">
         <v>116</v>
       </c>
-      <c r="E37" s="166" t="s">
+      <c r="E37" s="142" t="s">
         <v>40</v>
       </c>
-      <c r="F37" s="167">
+      <c r="F37" s="143">
         <v>44077</v>
       </c>
-      <c r="G37" s="167">
+      <c r="G37" s="143">
         <v>44107</v>
       </c>
-      <c r="H37" s="167"/>
-      <c r="I37" s="168">
-        <v>1</v>
-      </c>
-      <c r="J37" s="169">
-        <v>0</v>
+      <c r="H37" s="143">
+        <v>44107</v>
+      </c>
+      <c r="I37" s="144">
+        <v>1</v>
+      </c>
+      <c r="J37" s="145">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B38" s="132" t="s">
         <v>117</v>
       </c>
-      <c r="C38" s="165" t="s">
+      <c r="C38" s="141" t="s">
         <v>118</v>
       </c>
       <c r="D38" s="99" t="s">
         <v>119</v>
       </c>
-      <c r="E38" s="166" t="s">
+      <c r="E38" s="142" t="s">
         <v>82</v>
       </c>
-      <c r="F38" s="167">
+      <c r="F38" s="143">
         <v>44107</v>
       </c>
-      <c r="G38" s="167">
+      <c r="G38" s="143">
         <v>44138</v>
       </c>
-      <c r="H38" s="167"/>
-      <c r="I38" s="168">
-        <v>1</v>
-      </c>
-      <c r="J38" s="169">
-        <v>0</v>
+      <c r="H38" s="143">
+        <v>44168</v>
+      </c>
+      <c r="I38" s="144">
+        <v>1</v>
+      </c>
+      <c r="J38" s="145">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B39" s="132" t="s">
         <v>120</v>
       </c>
-      <c r="C39" s="165" t="s">
+      <c r="C39" s="141" t="s">
         <v>121</v>
       </c>
       <c r="D39" s="99" t="s">
         <v>122</v>
       </c>
-      <c r="E39" s="166" t="s">
+      <c r="E39" s="142" t="s">
         <v>82</v>
       </c>
-      <c r="F39" s="167">
+      <c r="F39" s="143">
         <v>44107</v>
       </c>
-      <c r="G39" s="167">
+      <c r="G39" s="143">
         <v>44138</v>
       </c>
-      <c r="H39" s="167"/>
-      <c r="I39" s="168">
-        <v>1</v>
-      </c>
-      <c r="J39" s="169">
+      <c r="H39" s="143">
+        <v>44168</v>
+      </c>
+      <c r="I39" s="144">
+        <v>1</v>
+      </c>
+      <c r="J39" s="145">
         <v>0</v>
       </c>
     </row>
@@ -5081,32 +5107,113 @@
       <c r="B40" s="132" t="s">
         <v>123</v>
       </c>
-      <c r="C40" s="165" t="s">
+      <c r="C40" s="141" t="s">
         <v>124</v>
       </c>
-      <c r="D40" s="165" t="s">
+      <c r="D40" s="141" t="s">
         <v>125</v>
       </c>
-      <c r="E40" s="166" t="s">
+      <c r="E40" s="142" t="s">
+        <v>59</v>
+      </c>
+      <c r="F40" s="143">
+        <v>44168</v>
+      </c>
+      <c r="G40" s="143" t="s">
+        <v>126</v>
+      </c>
+      <c r="H40" s="143"/>
+      <c r="I40" s="144">
+        <v>2</v>
+      </c>
+      <c r="J40" s="145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="132" t="s">
+        <v>127</v>
+      </c>
+      <c r="C41" s="141" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" s="141" t="s">
+        <v>128</v>
+      </c>
+      <c r="E41" s="142" t="s">
         <v>50</v>
       </c>
-      <c r="F40" s="167">
-        <v>44138</v>
-      </c>
-      <c r="G40" s="167">
+      <c r="F41" s="143">
         <v>44168</v>
       </c>
-      <c r="H40" s="167"/>
-      <c r="I40" s="168">
-        <v>1</v>
-      </c>
-      <c r="J40" s="169">
+      <c r="G41" s="143" t="s">
+        <v>126</v>
+      </c>
+      <c r="H41" s="143"/>
+      <c r="I41" s="144">
+        <v>2</v>
+      </c>
+      <c r="J41" s="145">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:10" ht="19.2" x14ac:dyDescent="0.35">
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B42" s="132" t="s">
+        <v>129</v>
+      </c>
+      <c r="C42" s="141" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="141" t="s">
+        <v>131</v>
+      </c>
+      <c r="E42" s="142" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" s="143">
+        <v>44168</v>
+      </c>
+      <c r="G42" s="143" t="s">
+        <v>126</v>
+      </c>
+      <c r="H42" s="143"/>
+      <c r="I42" s="144">
+        <v>2</v>
+      </c>
+      <c r="J42" s="145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="132" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="141" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" s="141" t="s">
+        <v>131</v>
+      </c>
+      <c r="E43" s="142" t="s">
+        <v>96</v>
+      </c>
+      <c r="F43" s="143">
+        <v>44168</v>
+      </c>
+      <c r="G43" s="143" t="s">
+        <v>126</v>
+      </c>
+      <c r="H43" s="143"/>
+      <c r="I43" s="144">
+        <v>2</v>
+      </c>
+      <c r="J43" s="145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" ht="19.2" x14ac:dyDescent="0.35">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -5183,7 +5290,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J35:J40">
+  <conditionalFormatting sqref="J35:J43">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="percent" val="0"/>
@@ -5275,7 +5382,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J35:J40</xm:sqref>
+          <xm:sqref>J35:J43</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>